<commit_message>
Update sales 23/24 resources
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-sales-specification-2023-24.xlsx
+++ b/public/files/bulk-upload-sales-specification-2023-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="443">
   <si>
     <t>Field number</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>Numeric, range 1 only</t>
-  </si>
-  <si>
-    <t>Yes, if buyer was not interviewed (if field 28 = 1)</t>
   </si>
   <si>
     <t>What is buyer 1’s age?</t>
@@ -3026,7 +3023,7 @@
         <v>118</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
@@ -3052,16 +3049,16 @@
         <v>30.0</v>
       </c>
       <c r="B79" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="D79" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="E79" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="80">
@@ -3069,23 +3066,23 @@
         <v>31.0</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D80" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
       <c r="C81" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E81" s="11"/>
     </row>
@@ -3093,7 +3090,7 @@
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
       <c r="C82" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E82" s="11"/>
     </row>
@@ -3101,7 +3098,7 @@
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="C83" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E83" s="11"/>
     </row>
@@ -3109,7 +3106,7 @@
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="12"/>
@@ -3119,23 +3116,23 @@
         <v>32.0</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
@@ -3144,7 +3141,7 @@
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
       <c r="C87" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
@@ -3153,7 +3150,7 @@
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
@@ -3162,7 +3159,7 @@
       <c r="A89" s="11"/>
       <c r="B89" s="11"/>
       <c r="C89" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
@@ -3171,7 +3168,7 @@
       <c r="A90" s="11"/>
       <c r="B90" s="11"/>
       <c r="C90" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
@@ -3180,7 +3177,7 @@
       <c r="A91" s="11"/>
       <c r="B91" s="11"/>
       <c r="C91" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
@@ -3189,7 +3186,7 @@
       <c r="A92" s="11"/>
       <c r="B92" s="11"/>
       <c r="C92" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
@@ -3198,7 +3195,7 @@
       <c r="A93" s="11"/>
       <c r="B93" s="11"/>
       <c r="C93" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
@@ -3207,7 +3204,7 @@
       <c r="A94" s="11"/>
       <c r="B94" s="11"/>
       <c r="C94" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
@@ -3216,7 +3213,7 @@
       <c r="A95" s="11"/>
       <c r="B95" s="11"/>
       <c r="C95" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
@@ -3225,7 +3222,7 @@
       <c r="A96" s="11"/>
       <c r="B96" s="11"/>
       <c r="C96" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -3234,7 +3231,7 @@
       <c r="A97" s="11"/>
       <c r="B97" s="11"/>
       <c r="C97" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -3243,7 +3240,7 @@
       <c r="A98" s="11"/>
       <c r="B98" s="11"/>
       <c r="C98" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
@@ -3252,7 +3249,7 @@
       <c r="A99" s="11"/>
       <c r="B99" s="11"/>
       <c r="C99" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
@@ -3261,7 +3258,7 @@
       <c r="A100" s="11"/>
       <c r="B100" s="11"/>
       <c r="C100" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
@@ -3270,7 +3267,7 @@
       <c r="A101" s="11"/>
       <c r="B101" s="11"/>
       <c r="C101" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
@@ -3279,7 +3276,7 @@
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
@@ -3288,7 +3285,7 @@
       <c r="A103" s="11"/>
       <c r="B103" s="11"/>
       <c r="C103" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
@@ -3297,7 +3294,7 @@
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
       <c r="C104" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -3307,23 +3304,23 @@
         <v>33.0</v>
       </c>
       <c r="B105" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C105" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="D105" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D105" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E105" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="11"/>
       <c r="B106" s="11"/>
       <c r="C106" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
@@ -3332,7 +3329,7 @@
       <c r="A107" s="11"/>
       <c r="B107" s="11"/>
       <c r="C107" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
@@ -3341,7 +3338,7 @@
       <c r="A108" s="11"/>
       <c r="B108" s="11"/>
       <c r="C108" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
@@ -3350,7 +3347,7 @@
       <c r="A109" s="11"/>
       <c r="B109" s="11"/>
       <c r="C109" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
@@ -3359,7 +3356,7 @@
       <c r="A110" s="12"/>
       <c r="B110" s="12"/>
       <c r="C110" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -3369,16 +3366,16 @@
         <v>34.0</v>
       </c>
       <c r="B111" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C111" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="D111" s="20" t="s">
         <v>97</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112">
@@ -3386,23 +3383,23 @@
         <v>35.0</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C112" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="11"/>
       <c r="B113" s="11"/>
       <c r="C113" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
@@ -3411,7 +3408,7 @@
       <c r="A114" s="11"/>
       <c r="B114" s="11"/>
       <c r="C114" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
@@ -3420,7 +3417,7 @@
       <c r="A115" s="11"/>
       <c r="B115" s="11"/>
       <c r="C115" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
@@ -3429,7 +3426,7 @@
       <c r="A116" s="11"/>
       <c r="B116" s="11"/>
       <c r="C116" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
@@ -3438,7 +3435,7 @@
       <c r="A117" s="11"/>
       <c r="B117" s="11"/>
       <c r="C117" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
@@ -3447,7 +3444,7 @@
       <c r="A118" s="11"/>
       <c r="B118" s="11"/>
       <c r="C118" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
@@ -3456,7 +3453,7 @@
       <c r="A119" s="11"/>
       <c r="B119" s="11"/>
       <c r="C119" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
@@ -3465,7 +3462,7 @@
       <c r="A120" s="11"/>
       <c r="B120" s="11"/>
       <c r="C120" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
@@ -3474,7 +3471,7 @@
       <c r="A121" s="11"/>
       <c r="B121" s="11"/>
       <c r="C121" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
@@ -3483,7 +3480,7 @@
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
@@ -3493,7 +3490,7 @@
         <v>36.0</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C123" s="17" t="s">
         <v>27</v>
@@ -3502,7 +3499,7 @@
         <v>62</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124">
@@ -3528,23 +3525,23 @@
         <v>37.0</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C126" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D126" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E126" s="40" t="s">
         <v>176</v>
-      </c>
-      <c r="E126" s="40" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="11"/>
       <c r="B127" s="11"/>
       <c r="C127" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
@@ -3553,7 +3550,7 @@
       <c r="A128" s="11"/>
       <c r="B128" s="11"/>
       <c r="C128" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
@@ -3562,7 +3559,7 @@
       <c r="A129" s="11"/>
       <c r="B129" s="11"/>
       <c r="C129" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
@@ -3571,7 +3568,7 @@
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
       <c r="C130" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
@@ -3581,16 +3578,16 @@
         <v>38.0</v>
       </c>
       <c r="B131" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C131" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C131" s="20" t="s">
+      <c r="D131" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="D131" s="20" t="s">
+      <c r="E131" s="26" t="s">
         <v>183</v>
-      </c>
-      <c r="E131" s="26" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="132">
@@ -3598,23 +3595,23 @@
         <v>39.0</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C132" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D132" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E132" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="11"/>
       <c r="B133" s="11"/>
       <c r="C133" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E133" s="11"/>
     </row>
@@ -3622,7 +3619,7 @@
       <c r="A134" s="11"/>
       <c r="B134" s="11"/>
       <c r="C134" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E134" s="11"/>
     </row>
@@ -3630,7 +3627,7 @@
       <c r="A135" s="11"/>
       <c r="B135" s="11"/>
       <c r="C135" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E135" s="11"/>
     </row>
@@ -3638,7 +3635,7 @@
       <c r="A136" s="12"/>
       <c r="B136" s="12"/>
       <c r="C136" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D136" s="35"/>
       <c r="E136" s="12"/>
@@ -3648,23 +3645,23 @@
         <v>40.0</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="11"/>
       <c r="B138" s="11"/>
       <c r="C138" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
@@ -3673,7 +3670,7 @@
       <c r="A139" s="11"/>
       <c r="B139" s="11"/>
       <c r="C139" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
@@ -3682,7 +3679,7 @@
       <c r="A140" s="11"/>
       <c r="B140" s="11"/>
       <c r="C140" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
@@ -3691,7 +3688,7 @@
       <c r="A141" s="11"/>
       <c r="B141" s="11"/>
       <c r="C141" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
@@ -3700,7 +3697,7 @@
       <c r="A142" s="11"/>
       <c r="B142" s="11"/>
       <c r="C142" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
@@ -3709,7 +3706,7 @@
       <c r="A143" s="11"/>
       <c r="B143" s="11"/>
       <c r="C143" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
@@ -3718,7 +3715,7 @@
       <c r="A144" s="11"/>
       <c r="B144" s="11"/>
       <c r="C144" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -3727,7 +3724,7 @@
       <c r="A145" s="11"/>
       <c r="B145" s="11"/>
       <c r="C145" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
@@ -3736,7 +3733,7 @@
       <c r="A146" s="11"/>
       <c r="B146" s="11"/>
       <c r="C146" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
@@ -3745,7 +3742,7 @@
       <c r="A147" s="11"/>
       <c r="B147" s="11"/>
       <c r="C147" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
@@ -3754,7 +3751,7 @@
       <c r="A148" s="11"/>
       <c r="B148" s="11"/>
       <c r="C148" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
@@ -3763,7 +3760,7 @@
       <c r="A149" s="11"/>
       <c r="B149" s="11"/>
       <c r="C149" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
@@ -3772,7 +3769,7 @@
       <c r="A150" s="11"/>
       <c r="B150" s="11"/>
       <c r="C150" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
@@ -3781,7 +3778,7 @@
       <c r="A151" s="11"/>
       <c r="B151" s="11"/>
       <c r="C151" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
@@ -3790,7 +3787,7 @@
       <c r="A152" s="11"/>
       <c r="B152" s="11"/>
       <c r="C152" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
@@ -3799,7 +3796,7 @@
       <c r="A153" s="11"/>
       <c r="B153" s="11"/>
       <c r="C153" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
@@ -3808,7 +3805,7 @@
       <c r="A154" s="11"/>
       <c r="B154" s="11"/>
       <c r="C154" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
@@ -3817,7 +3814,7 @@
       <c r="A155" s="11"/>
       <c r="B155" s="11"/>
       <c r="C155" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
@@ -3826,7 +3823,7 @@
       <c r="A156" s="12"/>
       <c r="B156" s="12"/>
       <c r="C156" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D156" s="12"/>
       <c r="E156" s="11"/>
@@ -3836,23 +3833,23 @@
         <v>41.0</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C157" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D157" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D157" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E157" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="11"/>
       <c r="B158" s="11"/>
       <c r="C158" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
@@ -3861,7 +3858,7 @@
       <c r="A159" s="11"/>
       <c r="B159" s="11"/>
       <c r="C159" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
@@ -3870,7 +3867,7 @@
       <c r="A160" s="11"/>
       <c r="B160" s="11"/>
       <c r="C160" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
@@ -3879,7 +3876,7 @@
       <c r="A161" s="11"/>
       <c r="B161" s="11"/>
       <c r="C161" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -3888,7 +3885,7 @@
       <c r="A162" s="12"/>
       <c r="B162" s="12"/>
       <c r="C162" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D162" s="12"/>
       <c r="E162" s="12"/>
@@ -3898,16 +3895,16 @@
         <v>42.0</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D163" s="20" t="s">
         <v>97</v>
       </c>
       <c r="E163" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="164">
@@ -3915,23 +3912,23 @@
         <v>43.0</v>
       </c>
       <c r="B164" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C164" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D164" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E164" s="40" t="s">
         <v>195</v>
-      </c>
-      <c r="E164" s="40" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="11"/>
       <c r="B165" s="11"/>
       <c r="C165" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
@@ -3940,7 +3937,7 @@
       <c r="A166" s="11"/>
       <c r="B166" s="11"/>
       <c r="C166" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
@@ -3949,7 +3946,7 @@
       <c r="A167" s="11"/>
       <c r="B167" s="11"/>
       <c r="C167" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
@@ -3958,7 +3955,7 @@
       <c r="A168" s="11"/>
       <c r="B168" s="11"/>
       <c r="C168" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
@@ -3967,7 +3964,7 @@
       <c r="A169" s="11"/>
       <c r="B169" s="11"/>
       <c r="C169" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
@@ -3976,7 +3973,7 @@
       <c r="A170" s="11"/>
       <c r="B170" s="11"/>
       <c r="C170" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
@@ -3985,7 +3982,7 @@
       <c r="A171" s="11"/>
       <c r="B171" s="11"/>
       <c r="C171" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
@@ -3994,7 +3991,7 @@
       <c r="A172" s="11"/>
       <c r="B172" s="11"/>
       <c r="C172" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
@@ -4003,7 +4000,7 @@
       <c r="A173" s="11"/>
       <c r="B173" s="11"/>
       <c r="C173" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
@@ -4012,7 +4009,7 @@
       <c r="A174" s="11"/>
       <c r="B174" s="11"/>
       <c r="C174" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
@@ -4021,7 +4018,7 @@
       <c r="A175" s="12"/>
       <c r="B175" s="12"/>
       <c r="C175" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
@@ -4031,7 +4028,7 @@
         <v>44.0</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C176" s="17" t="s">
         <v>27</v>
@@ -4040,7 +4037,7 @@
         <v>62</v>
       </c>
       <c r="E176" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="177">
@@ -4066,16 +4063,16 @@
         <v>45.0</v>
       </c>
       <c r="B179" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C179" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C179" s="8" t="s">
+      <c r="D179" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D179" s="8" t="s">
-        <v>201</v>
-      </c>
       <c r="E179" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="180">
@@ -4083,23 +4080,23 @@
         <v>46.0</v>
       </c>
       <c r="B180" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C180" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D180" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E180" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="11"/>
       <c r="B181" s="11"/>
       <c r="C181" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
@@ -4108,7 +4105,7 @@
       <c r="A182" s="11"/>
       <c r="B182" s="11"/>
       <c r="C182" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
@@ -4117,7 +4114,7 @@
       <c r="A183" s="11"/>
       <c r="B183" s="11"/>
       <c r="C183" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
@@ -4126,7 +4123,7 @@
       <c r="A184" s="12"/>
       <c r="B184" s="12"/>
       <c r="C184" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D184" s="12"/>
       <c r="E184" s="12"/>
@@ -4136,16 +4133,16 @@
         <v>47.0</v>
       </c>
       <c r="B185" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C185" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C185" s="20" t="s">
+      <c r="D185" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D185" s="8" t="s">
+      <c r="E185" s="42" t="s">
         <v>207</v>
-      </c>
-      <c r="E185" s="42" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="186">
@@ -4153,36 +4150,36 @@
         <v>48.0</v>
       </c>
       <c r="B186" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C186" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D186" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E186" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="187">
       <c r="B187" s="11"/>
       <c r="C187" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E187" s="11"/>
     </row>
     <row r="188">
       <c r="B188" s="11"/>
       <c r="C188" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E188" s="11"/>
     </row>
     <row r="189">
       <c r="B189" s="11"/>
       <c r="C189" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E189" s="11"/>
     </row>
@@ -4190,7 +4187,7 @@
       <c r="A190" s="35"/>
       <c r="B190" s="12"/>
       <c r="C190" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="12"/>
@@ -4200,23 +4197,23 @@
         <v>49.0</v>
       </c>
       <c r="B191" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C191" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E191" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="11"/>
       <c r="B192" s="11"/>
       <c r="C192" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
@@ -4225,7 +4222,7 @@
       <c r="A193" s="11"/>
       <c r="B193" s="11"/>
       <c r="C193" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
@@ -4234,7 +4231,7 @@
       <c r="A194" s="11"/>
       <c r="B194" s="11"/>
       <c r="C194" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
@@ -4243,7 +4240,7 @@
       <c r="A195" s="11"/>
       <c r="B195" s="11"/>
       <c r="C195" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
@@ -4252,7 +4249,7 @@
       <c r="A196" s="11"/>
       <c r="B196" s="11"/>
       <c r="C196" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
@@ -4261,7 +4258,7 @@
       <c r="A197" s="11"/>
       <c r="B197" s="11"/>
       <c r="C197" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
@@ -4270,7 +4267,7 @@
       <c r="A198" s="11"/>
       <c r="B198" s="11"/>
       <c r="C198" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
@@ -4279,7 +4276,7 @@
       <c r="A199" s="11"/>
       <c r="B199" s="11"/>
       <c r="C199" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
@@ -4288,7 +4285,7 @@
       <c r="A200" s="11"/>
       <c r="B200" s="11"/>
       <c r="C200" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
@@ -4297,7 +4294,7 @@
       <c r="A201" s="11"/>
       <c r="B201" s="11"/>
       <c r="C201" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
@@ -4306,7 +4303,7 @@
       <c r="A202" s="12"/>
       <c r="B202" s="12"/>
       <c r="C202" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D202" s="12"/>
       <c r="E202" s="12"/>
@@ -4316,22 +4313,22 @@
         <v>50.0</v>
       </c>
       <c r="B203" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C203" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D203" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E203" s="40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204">
       <c r="B204" s="11"/>
       <c r="C204" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
@@ -4339,7 +4336,7 @@
     <row r="205">
       <c r="B205" s="11"/>
       <c r="C205" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
@@ -4347,7 +4344,7 @@
     <row r="206">
       <c r="B206" s="11"/>
       <c r="C206" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
@@ -4356,7 +4353,7 @@
       <c r="A207" s="35"/>
       <c r="B207" s="12"/>
       <c r="C207" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D207" s="12"/>
       <c r="E207" s="12"/>
@@ -4366,16 +4363,16 @@
         <v>51.0</v>
       </c>
       <c r="B208" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C208" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D208" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E208" s="42" t="s">
         <v>217</v>
-      </c>
-      <c r="C208" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D208" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E208" s="42" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="209">
@@ -4383,43 +4380,43 @@
         <v>52.0</v>
       </c>
       <c r="B209" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C209" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E209" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="210">
       <c r="B210" s="11"/>
       <c r="C210" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E210" s="11"/>
     </row>
     <row r="211">
       <c r="B211" s="11"/>
       <c r="C211" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E211" s="11"/>
     </row>
     <row r="212">
       <c r="B212" s="11"/>
       <c r="C212" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E212" s="11"/>
     </row>
     <row r="213">
       <c r="B213" s="12"/>
       <c r="C213" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="12"/>
@@ -4429,22 +4426,22 @@
         <v>53.0</v>
       </c>
       <c r="B214" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C214" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E214" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="215">
       <c r="B215" s="11"/>
       <c r="C215" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
@@ -4452,7 +4449,7 @@
     <row r="216">
       <c r="B216" s="11"/>
       <c r="C216" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
@@ -4460,7 +4457,7 @@
     <row r="217">
       <c r="B217" s="11"/>
       <c r="C217" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
@@ -4468,7 +4465,7 @@
     <row r="218">
       <c r="B218" s="11"/>
       <c r="C218" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
@@ -4476,7 +4473,7 @@
     <row r="219">
       <c r="B219" s="11"/>
       <c r="C219" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
@@ -4484,7 +4481,7 @@
     <row r="220">
       <c r="B220" s="11"/>
       <c r="C220" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
@@ -4492,7 +4489,7 @@
     <row r="221">
       <c r="B221" s="11"/>
       <c r="C221" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
@@ -4500,7 +4497,7 @@
     <row r="222">
       <c r="B222" s="11"/>
       <c r="C222" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
@@ -4508,7 +4505,7 @@
     <row r="223">
       <c r="B223" s="11"/>
       <c r="C223" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
@@ -4516,7 +4513,7 @@
     <row r="224">
       <c r="B224" s="11"/>
       <c r="C224" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
@@ -4524,7 +4521,7 @@
     <row r="225">
       <c r="B225" s="12"/>
       <c r="C225" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D225" s="12"/>
       <c r="E225" s="12"/>
@@ -4534,22 +4531,22 @@
         <v>54.0</v>
       </c>
       <c r="B226" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C226" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D226" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E226" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="227">
       <c r="B227" s="11"/>
       <c r="C227" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
@@ -4557,7 +4554,7 @@
     <row r="228">
       <c r="B228" s="11"/>
       <c r="C228" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
@@ -4565,7 +4562,7 @@
     <row r="229">
       <c r="B229" s="11"/>
       <c r="C229" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
@@ -4574,7 +4571,7 @@
       <c r="A230" s="35"/>
       <c r="B230" s="12"/>
       <c r="C230" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D230" s="12"/>
       <c r="E230" s="12"/>
@@ -4584,16 +4581,16 @@
         <v>55.0</v>
       </c>
       <c r="B231" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C231" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D231" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E231" s="42" t="s">
         <v>225</v>
-      </c>
-      <c r="C231" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D231" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E231" s="42" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="232">
@@ -4601,36 +4598,36 @@
         <v>56.0</v>
       </c>
       <c r="B232" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C232" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D232" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="233">
       <c r="B233" s="11"/>
       <c r="C233" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E233" s="11"/>
     </row>
     <row r="234">
       <c r="B234" s="11"/>
       <c r="C234" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E234" s="11"/>
     </row>
     <row r="235">
       <c r="B235" s="11"/>
       <c r="C235" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E235" s="11"/>
     </row>
@@ -4638,7 +4635,7 @@
       <c r="A236" s="35"/>
       <c r="B236" s="12"/>
       <c r="C236" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D236" s="35"/>
       <c r="E236" s="12"/>
@@ -4648,23 +4645,23 @@
         <v>57.0</v>
       </c>
       <c r="B237" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C237" s="46" t="s">
         <v>27</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E237" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="11"/>
       <c r="B238" s="11"/>
       <c r="C238" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
@@ -4673,7 +4670,7 @@
       <c r="A239" s="11"/>
       <c r="B239" s="11"/>
       <c r="C239" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
@@ -4682,7 +4679,7 @@
       <c r="A240" s="11"/>
       <c r="B240" s="11"/>
       <c r="C240" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
@@ -4691,7 +4688,7 @@
       <c r="A241" s="11"/>
       <c r="B241" s="11"/>
       <c r="C241" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
@@ -4700,7 +4697,7 @@
       <c r="A242" s="11"/>
       <c r="B242" s="11"/>
       <c r="C242" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
@@ -4709,7 +4706,7 @@
       <c r="A243" s="11"/>
       <c r="B243" s="11"/>
       <c r="C243" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
@@ -4718,7 +4715,7 @@
       <c r="A244" s="11"/>
       <c r="B244" s="11"/>
       <c r="C244" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D244" s="11"/>
       <c r="E244" s="11"/>
@@ -4727,7 +4724,7 @@
       <c r="A245" s="11"/>
       <c r="B245" s="11"/>
       <c r="C245" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
@@ -4736,7 +4733,7 @@
       <c r="A246" s="11"/>
       <c r="B246" s="11"/>
       <c r="C246" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
@@ -4745,7 +4742,7 @@
       <c r="A247" s="11"/>
       <c r="B247" s="11"/>
       <c r="C247" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
@@ -4754,7 +4751,7 @@
       <c r="A248" s="12"/>
       <c r="B248" s="12"/>
       <c r="C248" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D248" s="12"/>
       <c r="E248" s="12"/>
@@ -4764,22 +4761,22 @@
         <v>58.0</v>
       </c>
       <c r="B249" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C249" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D249" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E249" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="250">
       <c r="B250" s="11"/>
       <c r="C250" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D250" s="11"/>
       <c r="E250" s="18"/>
@@ -4787,7 +4784,7 @@
     <row r="251">
       <c r="B251" s="11"/>
       <c r="C251" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D251" s="11"/>
       <c r="E251" s="18"/>
@@ -4795,7 +4792,7 @@
     <row r="252">
       <c r="B252" s="11"/>
       <c r="C252" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D252" s="11"/>
       <c r="E252" s="18"/>
@@ -4803,7 +4800,7 @@
     <row r="253">
       <c r="B253" s="12"/>
       <c r="C253" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D253" s="12"/>
       <c r="E253" s="21"/>
@@ -4813,16 +4810,16 @@
         <v>59.0</v>
       </c>
       <c r="B254" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C254" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D254" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C254" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D254" s="20" t="s">
+      <c r="E254" s="49" t="s">
         <v>234</v>
-      </c>
-      <c r="E254" s="49" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="255">
@@ -4830,22 +4827,22 @@
         <v>60.0</v>
       </c>
       <c r="B255" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C255" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D255" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E255" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="256">
       <c r="B256" s="11"/>
       <c r="C256" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D256" s="11"/>
       <c r="E256" s="18"/>
@@ -4853,7 +4850,7 @@
     <row r="257">
       <c r="B257" s="11"/>
       <c r="C257" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D257" s="11"/>
       <c r="E257" s="18"/>
@@ -4861,7 +4858,7 @@
     <row r="258">
       <c r="B258" s="11"/>
       <c r="C258" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D258" s="11"/>
       <c r="E258" s="18"/>
@@ -4869,7 +4866,7 @@
     <row r="259">
       <c r="B259" s="12"/>
       <c r="C259" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D259" s="12"/>
       <c r="E259" s="21"/>
@@ -4879,23 +4876,23 @@
         <v>61.0</v>
       </c>
       <c r="B260" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C260" s="50" t="s">
         <v>27</v>
       </c>
       <c r="D260" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E260" s="48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="11"/>
       <c r="B261" s="11"/>
       <c r="C261" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D261" s="11"/>
       <c r="E261" s="18"/>
@@ -4904,7 +4901,7 @@
       <c r="A262" s="11"/>
       <c r="B262" s="11"/>
       <c r="C262" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D262" s="11"/>
       <c r="E262" s="18"/>
@@ -4913,7 +4910,7 @@
       <c r="A263" s="11"/>
       <c r="B263" s="11"/>
       <c r="C263" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D263" s="11"/>
       <c r="E263" s="18"/>
@@ -4922,7 +4919,7 @@
       <c r="A264" s="11"/>
       <c r="B264" s="11"/>
       <c r="C264" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D264" s="11"/>
       <c r="E264" s="18"/>
@@ -4931,7 +4928,7 @@
       <c r="A265" s="11"/>
       <c r="B265" s="11"/>
       <c r="C265" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D265" s="11"/>
       <c r="E265" s="18"/>
@@ -4940,7 +4937,7 @@
       <c r="A266" s="11"/>
       <c r="B266" s="11"/>
       <c r="C266" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D266" s="11"/>
       <c r="E266" s="18"/>
@@ -4949,7 +4946,7 @@
       <c r="A267" s="11"/>
       <c r="B267" s="11"/>
       <c r="C267" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D267" s="11"/>
       <c r="E267" s="18"/>
@@ -4958,7 +4955,7 @@
       <c r="A268" s="11"/>
       <c r="B268" s="11"/>
       <c r="C268" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D268" s="11"/>
       <c r="E268" s="18"/>
@@ -4967,7 +4964,7 @@
       <c r="A269" s="11"/>
       <c r="B269" s="11"/>
       <c r="C269" s="52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D269" s="11"/>
       <c r="E269" s="18"/>
@@ -4976,7 +4973,7 @@
       <c r="A270" s="11"/>
       <c r="B270" s="11"/>
       <c r="C270" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D270" s="11"/>
       <c r="E270" s="18"/>
@@ -4985,14 +4982,14 @@
       <c r="A271" s="12"/>
       <c r="B271" s="12"/>
       <c r="C271" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D271" s="12"/>
       <c r="E271" s="21"/>
     </row>
     <row r="272" ht="24.75" customHeight="1">
       <c r="A272" s="54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B272" s="4"/>
       <c r="C272" s="4"/>
@@ -5004,13 +5001,13 @@
         <v>62.0</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E273" s="10" t="s">
         <v>9</v>
@@ -5020,7 +5017,7 @@
       <c r="A274" s="11"/>
       <c r="B274" s="11"/>
       <c r="C274" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D274" s="11"/>
       <c r="E274" s="11"/>
@@ -5029,7 +5026,7 @@
       <c r="A275" s="11"/>
       <c r="B275" s="11"/>
       <c r="C275" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D275" s="11"/>
       <c r="E275" s="11"/>
@@ -5038,7 +5035,7 @@
       <c r="A276" s="11"/>
       <c r="B276" s="11"/>
       <c r="C276" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D276" s="11"/>
       <c r="E276" s="11"/>
@@ -5047,7 +5044,7 @@
       <c r="A277" s="11"/>
       <c r="B277" s="11"/>
       <c r="C277" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D277" s="11"/>
       <c r="E277" s="11"/>
@@ -5056,7 +5053,7 @@
       <c r="A278" s="11"/>
       <c r="B278" s="11"/>
       <c r="C278" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D278" s="11"/>
       <c r="E278" s="11"/>
@@ -5065,7 +5062,7 @@
       <c r="A279" s="11"/>
       <c r="B279" s="11"/>
       <c r="C279" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D279" s="11"/>
       <c r="E279" s="11"/>
@@ -5074,7 +5071,7 @@
       <c r="A280" s="11"/>
       <c r="B280" s="11"/>
       <c r="C280" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D280" s="11"/>
       <c r="E280" s="11"/>
@@ -5092,7 +5089,7 @@
       <c r="A282" s="12"/>
       <c r="B282" s="12"/>
       <c r="C282" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D282" s="12"/>
       <c r="E282" s="12"/>
@@ -5102,13 +5099,13 @@
         <v>63.0</v>
       </c>
       <c r="B283" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C283" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="C283" s="17" t="s">
+      <c r="D283" s="17" t="s">
         <v>252</v>
-      </c>
-      <c r="D283" s="17" t="s">
-        <v>253</v>
       </c>
       <c r="E283" s="10" t="s">
         <v>9</v>
@@ -5146,23 +5143,23 @@
         <v>64.0</v>
       </c>
       <c r="B287" s="56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C287" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D287" s="58" t="s">
         <v>102</v>
       </c>
       <c r="E287" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="12"/>
       <c r="B288" s="35"/>
       <c r="C288" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D288" s="18"/>
       <c r="E288" s="11"/>
@@ -5172,10 +5169,10 @@
         <v>65.0</v>
       </c>
       <c r="B289" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C289" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D289" s="58" t="s">
         <v>106</v>
@@ -5186,7 +5183,7 @@
       <c r="A290" s="12"/>
       <c r="B290" s="19"/>
       <c r="C290" s="61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D290" s="18"/>
       <c r="E290" s="12"/>
@@ -5196,10 +5193,10 @@
         <v>66.0</v>
       </c>
       <c r="B291" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D291" s="15" t="s">
         <v>109</v>
@@ -5212,7 +5209,7 @@
       <c r="A292" s="12"/>
       <c r="B292" s="19"/>
       <c r="C292" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D292" s="21"/>
       <c r="E292" s="12"/>
@@ -5222,13 +5219,13 @@
         <v>67.0</v>
       </c>
       <c r="B293" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C293" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D293" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E293" s="27" t="s">
         <v>13</v>
@@ -5247,7 +5244,7 @@
       <c r="A295" s="12"/>
       <c r="B295" s="12"/>
       <c r="C295" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D295" s="12"/>
       <c r="E295" s="11"/>
@@ -5257,13 +5254,13 @@
         <v>68.0</v>
       </c>
       <c r="B296" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C296" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D296" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E296" s="11"/>
     </row>
@@ -5280,7 +5277,7 @@
       <c r="A298" s="12"/>
       <c r="B298" s="12"/>
       <c r="C298" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D298" s="12"/>
       <c r="E298" s="11"/>
@@ -5290,13 +5287,13 @@
         <v>69.0</v>
       </c>
       <c r="B299" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C299" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D299" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E299" s="11"/>
     </row>
@@ -5313,7 +5310,7 @@
       <c r="A301" s="12"/>
       <c r="B301" s="12"/>
       <c r="C301" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D301" s="12"/>
       <c r="E301" s="11"/>
@@ -5323,13 +5320,13 @@
         <v>70.0</v>
       </c>
       <c r="B302" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C302" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D302" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E302" s="11"/>
     </row>
@@ -5346,7 +5343,7 @@
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
       <c r="C304" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D304" s="12"/>
       <c r="E304" s="12"/>
@@ -5356,7 +5353,7 @@
         <v>71.0</v>
       </c>
       <c r="B305" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C305" s="17" t="s">
         <v>27</v>
@@ -5365,7 +5362,7 @@
         <v>26</v>
       </c>
       <c r="E305" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="306">
@@ -5400,23 +5397,23 @@
         <v>72.0</v>
       </c>
       <c r="B309" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C309" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E309" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="11"/>
       <c r="B310" s="11"/>
       <c r="C310" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D310" s="11"/>
       <c r="E310" s="11"/>
@@ -5425,7 +5422,7 @@
       <c r="A311" s="11"/>
       <c r="B311" s="11"/>
       <c r="C311" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D311" s="11"/>
       <c r="E311" s="11"/>
@@ -5434,7 +5431,7 @@
       <c r="A312" s="11"/>
       <c r="B312" s="11"/>
       <c r="C312" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D312" s="11"/>
       <c r="E312" s="11"/>
@@ -5443,7 +5440,7 @@
       <c r="A313" s="11"/>
       <c r="B313" s="11"/>
       <c r="C313" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D313" s="11"/>
       <c r="E313" s="11"/>
@@ -5452,7 +5449,7 @@
       <c r="A314" s="11"/>
       <c r="B314" s="11"/>
       <c r="C314" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D314" s="11"/>
       <c r="E314" s="11"/>
@@ -5461,7 +5458,7 @@
       <c r="A315" s="11"/>
       <c r="B315" s="11"/>
       <c r="C315" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D315" s="11"/>
       <c r="E315" s="11"/>
@@ -5470,7 +5467,7 @@
       <c r="A316" s="11"/>
       <c r="B316" s="11"/>
       <c r="C316" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D316" s="11"/>
       <c r="E316" s="11"/>
@@ -5488,14 +5485,14 @@
       <c r="A318" s="12"/>
       <c r="B318" s="11"/>
       <c r="C318" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D318" s="11"/>
       <c r="E318" s="12"/>
     </row>
     <row r="319" ht="24.75" customHeight="1">
       <c r="A319" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -5507,13 +5504,13 @@
         <v>73.0</v>
       </c>
       <c r="B320" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C320" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="C320" s="36" t="s">
+      <c r="D320" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="D320" s="9" t="s">
-        <v>274</v>
       </c>
       <c r="E320" s="10" t="s">
         <v>9</v>
@@ -5541,7 +5538,7 @@
       <c r="A323" s="11"/>
       <c r="B323" s="11"/>
       <c r="C323" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D323" s="11"/>
       <c r="E323" s="11"/>
@@ -5550,7 +5547,7 @@
       <c r="A324" s="11"/>
       <c r="B324" s="11"/>
       <c r="C324" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D324" s="11"/>
       <c r="E324" s="11"/>
@@ -5559,7 +5556,7 @@
       <c r="A325" s="11"/>
       <c r="B325" s="11"/>
       <c r="C325" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D325" s="11"/>
       <c r="E325" s="11"/>
@@ -5569,23 +5566,23 @@
         <v>74.0</v>
       </c>
       <c r="B326" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C326" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C326" s="9" t="s">
+      <c r="D326" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="D326" s="9" t="s">
+      <c r="E326" s="10" t="s">
         <v>280</v>
-      </c>
-      <c r="E326" s="10" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="11"/>
       <c r="B327" s="11"/>
       <c r="C327" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D327" s="11"/>
       <c r="E327" s="11"/>
@@ -5594,7 +5591,7 @@
       <c r="A328" s="11"/>
       <c r="B328" s="11"/>
       <c r="C328" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D328" s="11"/>
       <c r="E328" s="11"/>
@@ -5604,13 +5601,13 @@
         <v>75.0</v>
       </c>
       <c r="B329" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C329" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="D329" s="9" t="s">
         <v>284</v>
-      </c>
-      <c r="C329" s="56" t="s">
-        <v>273</v>
-      </c>
-      <c r="D329" s="9" t="s">
-        <v>285</v>
       </c>
       <c r="E329" s="10" t="s">
         <v>9</v>
@@ -5629,7 +5626,7 @@
       <c r="A331" s="11"/>
       <c r="B331" s="11"/>
       <c r="C331" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D331" s="11"/>
       <c r="E331" s="11"/>
@@ -5638,7 +5635,7 @@
       <c r="A332" s="11"/>
       <c r="B332" s="11"/>
       <c r="C332" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D332" s="11"/>
       <c r="E332" s="11"/>
@@ -5647,7 +5644,7 @@
       <c r="A333" s="11"/>
       <c r="B333" s="11"/>
       <c r="C333" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D333" s="11"/>
       <c r="E333" s="11"/>
@@ -5656,7 +5653,7 @@
       <c r="A334" s="11"/>
       <c r="B334" s="11"/>
       <c r="C334" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D334" s="11"/>
       <c r="E334" s="11"/>
@@ -5666,10 +5663,10 @@
         <v>76.0</v>
       </c>
       <c r="B335" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C335" s="17" t="s">
         <v>290</v>
-      </c>
-      <c r="C335" s="17" t="s">
-        <v>291</v>
       </c>
       <c r="D335" s="9" t="s">
         <v>26</v>
@@ -5719,10 +5716,10 @@
         <v>77.0</v>
       </c>
       <c r="B340" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C340" s="17" t="s">
         <v>292</v>
-      </c>
-      <c r="C340" s="17" t="s">
-        <v>293</v>
       </c>
       <c r="D340" s="11"/>
       <c r="E340" s="11"/>
@@ -5765,7 +5762,7 @@
     </row>
     <row r="345" ht="24.75" customHeight="1">
       <c r="A345" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -5777,13 +5774,13 @@
         <v>78.0</v>
       </c>
       <c r="B346" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C346" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C346" s="9" t="s">
+      <c r="D346" s="15" t="s">
         <v>296</v>
-      </c>
-      <c r="D346" s="15" t="s">
-        <v>297</v>
       </c>
       <c r="E346" s="27" t="s">
         <v>9</v>
@@ -5793,7 +5790,7 @@
       <c r="A347" s="12"/>
       <c r="B347" s="19"/>
       <c r="C347" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D347" s="18"/>
       <c r="E347" s="12"/>
@@ -5803,7 +5800,7 @@
         <v>79.0</v>
       </c>
       <c r="B348" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C348" s="9" t="s">
         <v>27</v>
@@ -5812,7 +5809,7 @@
         <v>62</v>
       </c>
       <c r="E348" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="349">
@@ -5838,23 +5835,23 @@
         <v>80.0</v>
       </c>
       <c r="B351" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C351" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D351" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="D351" s="15" t="s">
-        <v>297</v>
-      </c>
       <c r="E351" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="12"/>
       <c r="B352" s="19"/>
       <c r="C352" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D352" s="18"/>
       <c r="E352" s="12"/>
@@ -5864,7 +5861,7 @@
         <v>81.0</v>
       </c>
       <c r="B353" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C353" s="9" t="s">
         <v>27</v>
@@ -5873,7 +5870,7 @@
         <v>62</v>
       </c>
       <c r="E353" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="354">
@@ -5899,13 +5896,13 @@
         <v>82.0</v>
       </c>
       <c r="B356" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C356" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E356" s="10" t="s">
         <v>9</v>
@@ -5915,7 +5912,7 @@
       <c r="A357" s="11"/>
       <c r="B357" s="11"/>
       <c r="C357" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D357" s="11"/>
       <c r="E357" s="11"/>
@@ -5924,7 +5921,7 @@
       <c r="A358" s="11"/>
       <c r="B358" s="11"/>
       <c r="C358" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D358" s="11"/>
       <c r="E358" s="11"/>
@@ -5933,7 +5930,7 @@
       <c r="A359" s="11"/>
       <c r="B359" s="11"/>
       <c r="C359" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D359" s="11"/>
       <c r="E359" s="11"/>
@@ -5942,7 +5939,7 @@
       <c r="A360" s="12"/>
       <c r="B360" s="12"/>
       <c r="C360" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D360" s="12"/>
       <c r="E360" s="12"/>
@@ -5952,13 +5949,13 @@
         <v>83.0</v>
       </c>
       <c r="B361" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C361" s="64" t="s">
         <v>310</v>
       </c>
-      <c r="C361" s="64" t="s">
+      <c r="D361" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="D361" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="E361" s="6" t="s">
         <v>9</v>
@@ -5969,7 +5966,7 @@
         <v>84.0</v>
       </c>
       <c r="B362" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C362" s="17" t="s">
         <v>27</v>
@@ -6013,16 +6010,16 @@
         <v>85.0</v>
       </c>
       <c r="B366" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C366" s="17" t="s">
         <v>314</v>
-      </c>
-      <c r="C366" s="17" t="s">
-        <v>315</v>
       </c>
       <c r="D366" s="65" t="s">
         <v>26</v>
       </c>
       <c r="E366" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="367">
@@ -6059,7 +6056,7 @@
     </row>
     <row r="371" ht="24.75" customHeight="1">
       <c r="A371" s="66" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -6071,13 +6068,13 @@
         <v>86.0</v>
       </c>
       <c r="B372" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C372" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C372" s="9" t="s">
+      <c r="D372" s="15" t="s">
         <v>319</v>
-      </c>
-      <c r="D372" s="15" t="s">
-        <v>320</v>
       </c>
       <c r="E372" s="10" t="s">
         <v>33</v>
@@ -6087,7 +6084,7 @@
       <c r="A373" s="12"/>
       <c r="B373" s="12"/>
       <c r="C373" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D373" s="21"/>
       <c r="E373" s="12"/>
@@ -6097,10 +6094,10 @@
         <v>87.0</v>
       </c>
       <c r="B374" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C374" s="17" t="s">
         <v>322</v>
-      </c>
-      <c r="C374" s="17" t="s">
-        <v>323</v>
       </c>
       <c r="D374" s="9" t="s">
         <v>69</v>
@@ -6150,16 +6147,16 @@
         <v>88.0</v>
       </c>
       <c r="B379" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C379" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C379" s="8" t="s">
+      <c r="D379" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D379" s="8" t="s">
+      <c r="E379" s="10" t="s">
         <v>326</v>
-      </c>
-      <c r="E379" s="10" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="380">
@@ -6167,13 +6164,13 @@
         <v>89.0</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C380" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D380" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="D380" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="E380" s="11"/>
     </row>
@@ -6182,7 +6179,7 @@
         <v>90.0</v>
       </c>
       <c r="B381" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C381" s="17" t="s">
         <v>27</v>
@@ -6221,16 +6218,16 @@
         <v>91.0</v>
       </c>
       <c r="B385" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C385" s="17" t="s">
         <v>330</v>
-      </c>
-      <c r="C385" s="17" t="s">
-        <v>331</v>
       </c>
       <c r="D385" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E385" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="386">
@@ -6265,16 +6262,16 @@
         <v>92.0</v>
       </c>
       <c r="B389" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C389" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="C389" s="9" t="s">
-        <v>334</v>
       </c>
       <c r="D389" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E389" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="390">
@@ -6308,7 +6305,7 @@
         <v>19</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E392" s="11"/>
     </row>
@@ -6317,10 +6314,10 @@
         <v>95.0</v>
       </c>
       <c r="B393" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C393" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="C393" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="D393" s="9" t="s">
         <v>16</v>
@@ -6358,7 +6355,7 @@
         <v>19</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E396" s="12"/>
     </row>
@@ -6367,10 +6364,10 @@
         <v>98.0</v>
       </c>
       <c r="B397" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C397" s="9" t="s">
         <v>339</v>
-      </c>
-      <c r="C397" s="9" t="s">
-        <v>340</v>
       </c>
       <c r="D397" s="17" t="s">
         <v>26</v>
@@ -6420,7 +6417,7 @@
         <v>99.0</v>
       </c>
       <c r="B402" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C402" s="17" t="s">
         <v>27</v>
@@ -6451,16 +6448,16 @@
         <v>100.0</v>
       </c>
       <c r="B405" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C405" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C405" s="8" t="s">
+      <c r="D405" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="D405" s="8" t="s">
+      <c r="E405" s="10" t="s">
         <v>344</v>
-      </c>
-      <c r="E405" s="10" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="406">
@@ -6468,7 +6465,7 @@
         <v>101.0</v>
       </c>
       <c r="B406" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C406" s="17" t="s">
         <v>27</v>
@@ -6528,13 +6525,13 @@
         <v>102.0</v>
       </c>
       <c r="B412" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C412" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D412" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E412" s="11"/>
     </row>
@@ -6542,7 +6539,7 @@
       <c r="A413" s="11"/>
       <c r="B413" s="11"/>
       <c r="C413" s="69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D413" s="11"/>
       <c r="E413" s="11"/>
@@ -6551,7 +6548,7 @@
       <c r="A414" s="11"/>
       <c r="B414" s="11"/>
       <c r="C414" s="69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D414" s="11"/>
       <c r="E414" s="11"/>
@@ -6560,7 +6557,7 @@
       <c r="A415" s="11"/>
       <c r="B415" s="11"/>
       <c r="C415" s="69" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D415" s="11"/>
       <c r="E415" s="11"/>
@@ -6578,7 +6575,7 @@
       <c r="A417" s="12"/>
       <c r="B417" s="12"/>
       <c r="C417" s="69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D417" s="12"/>
       <c r="E417" s="12"/>
@@ -6588,13 +6585,13 @@
         <v>103.0</v>
       </c>
       <c r="B418" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C418" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C418" s="9" t="s">
+      <c r="D418" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D418" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E418" s="10" t="s">
         <v>33</v>
@@ -6604,7 +6601,7 @@
       <c r="A419" s="11"/>
       <c r="B419" s="16"/>
       <c r="C419" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D419" s="18"/>
       <c r="E419" s="11"/>
@@ -6614,13 +6611,13 @@
         <v>104.0</v>
       </c>
       <c r="B420" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C420" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="C420" s="9" t="s">
-        <v>358</v>
-      </c>
       <c r="D420" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E420" s="11"/>
     </row>
@@ -6628,7 +6625,7 @@
       <c r="A421" s="11"/>
       <c r="B421" s="11"/>
       <c r="C421" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D421" s="11"/>
       <c r="E421" s="11"/>
@@ -6638,7 +6635,7 @@
         <v>105.0</v>
       </c>
       <c r="B422" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C422" s="17" t="s">
         <v>27</v>
@@ -6671,16 +6668,16 @@
         <v>106.0</v>
       </c>
       <c r="B425" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C425" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="C425" s="9" t="s">
+      <c r="D425" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E425" s="6" t="s">
         <v>362</v>
-      </c>
-      <c r="D425" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="E425" s="6" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="426">
@@ -6688,23 +6685,23 @@
         <v>107.0</v>
       </c>
       <c r="B426" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C426" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D426" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E426" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="11"/>
       <c r="B427" s="11"/>
       <c r="C427" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D427" s="11"/>
       <c r="E427" s="11"/>
@@ -6713,7 +6710,7 @@
       <c r="A428" s="11"/>
       <c r="B428" s="11"/>
       <c r="C428" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D428" s="11"/>
       <c r="E428" s="11"/>
@@ -6722,7 +6719,7 @@
       <c r="A429" s="11"/>
       <c r="B429" s="11"/>
       <c r="C429" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D429" s="11"/>
       <c r="E429" s="11"/>
@@ -6731,7 +6728,7 @@
       <c r="A430" s="11"/>
       <c r="B430" s="11"/>
       <c r="C430" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D430" s="11"/>
       <c r="E430" s="11"/>
@@ -6740,7 +6737,7 @@
       <c r="A431" s="11"/>
       <c r="B431" s="11"/>
       <c r="C431" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D431" s="11"/>
       <c r="E431" s="11"/>
@@ -6749,7 +6746,7 @@
       <c r="A432" s="11"/>
       <c r="B432" s="11"/>
       <c r="C432" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D432" s="11"/>
       <c r="E432" s="11"/>
@@ -6758,7 +6755,7 @@
       <c r="A433" s="11"/>
       <c r="B433" s="11"/>
       <c r="C433" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D433" s="11"/>
       <c r="E433" s="11"/>
@@ -6767,7 +6764,7 @@
       <c r="A434" s="11"/>
       <c r="B434" s="11"/>
       <c r="C434" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D434" s="11"/>
       <c r="E434" s="11"/>
@@ -6776,7 +6773,7 @@
       <c r="A435" s="11"/>
       <c r="B435" s="11"/>
       <c r="C435" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D435" s="11"/>
       <c r="E435" s="11"/>
@@ -6785,7 +6782,7 @@
       <c r="A436" s="11"/>
       <c r="B436" s="11"/>
       <c r="C436" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D436" s="11"/>
       <c r="E436" s="11"/>
@@ -6794,7 +6791,7 @@
       <c r="A437" s="11"/>
       <c r="B437" s="11"/>
       <c r="C437" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D437" s="11"/>
       <c r="E437" s="11"/>
@@ -6803,7 +6800,7 @@
       <c r="A438" s="11"/>
       <c r="B438" s="11"/>
       <c r="C438" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D438" s="11"/>
       <c r="E438" s="11"/>
@@ -6812,7 +6809,7 @@
       <c r="A439" s="11"/>
       <c r="B439" s="11"/>
       <c r="C439" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D439" s="11"/>
       <c r="E439" s="11"/>
@@ -6821,7 +6818,7 @@
       <c r="A440" s="11"/>
       <c r="B440" s="11"/>
       <c r="C440" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D440" s="11"/>
       <c r="E440" s="11"/>
@@ -6830,7 +6827,7 @@
       <c r="A441" s="11"/>
       <c r="B441" s="11"/>
       <c r="C441" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D441" s="11"/>
       <c r="E441" s="11"/>
@@ -6839,7 +6836,7 @@
       <c r="A442" s="11"/>
       <c r="B442" s="11"/>
       <c r="C442" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D442" s="11"/>
       <c r="E442" s="11"/>
@@ -6848,7 +6845,7 @@
       <c r="A443" s="11"/>
       <c r="B443" s="11"/>
       <c r="C443" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D443" s="11"/>
       <c r="E443" s="11"/>
@@ -6857,7 +6854,7 @@
       <c r="A444" s="11"/>
       <c r="B444" s="11"/>
       <c r="C444" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D444" s="11"/>
       <c r="E444" s="11"/>
@@ -6866,7 +6863,7 @@
       <c r="A445" s="11"/>
       <c r="B445" s="11"/>
       <c r="C445" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D445" s="11"/>
       <c r="E445" s="11"/>
@@ -6875,7 +6872,7 @@
       <c r="A446" s="11"/>
       <c r="B446" s="11"/>
       <c r="C446" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D446" s="11"/>
       <c r="E446" s="11"/>
@@ -6884,7 +6881,7 @@
       <c r="A447" s="11"/>
       <c r="B447" s="11"/>
       <c r="C447" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D447" s="11"/>
       <c r="E447" s="11"/>
@@ -6893,7 +6890,7 @@
       <c r="A448" s="11"/>
       <c r="B448" s="11"/>
       <c r="C448" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D448" s="11"/>
       <c r="E448" s="11"/>
@@ -6902,7 +6899,7 @@
       <c r="A449" s="11"/>
       <c r="B449" s="11"/>
       <c r="C449" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D449" s="11"/>
       <c r="E449" s="11"/>
@@ -6911,7 +6908,7 @@
       <c r="A450" s="11"/>
       <c r="B450" s="11"/>
       <c r="C450" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D450" s="11"/>
       <c r="E450" s="11"/>
@@ -6920,7 +6917,7 @@
       <c r="A451" s="11"/>
       <c r="B451" s="11"/>
       <c r="C451" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D451" s="11"/>
       <c r="E451" s="11"/>
@@ -6929,7 +6926,7 @@
       <c r="A452" s="11"/>
       <c r="B452" s="11"/>
       <c r="C452" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D452" s="11"/>
       <c r="E452" s="11"/>
@@ -6938,7 +6935,7 @@
       <c r="A453" s="11"/>
       <c r="B453" s="11"/>
       <c r="C453" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D453" s="11"/>
       <c r="E453" s="11"/>
@@ -6947,7 +6944,7 @@
       <c r="A454" s="11"/>
       <c r="B454" s="11"/>
       <c r="C454" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D454" s="11"/>
       <c r="E454" s="11"/>
@@ -6956,7 +6953,7 @@
       <c r="A455" s="11"/>
       <c r="B455" s="11"/>
       <c r="C455" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D455" s="11"/>
       <c r="E455" s="11"/>
@@ -6965,7 +6962,7 @@
       <c r="A456" s="11"/>
       <c r="B456" s="11"/>
       <c r="C456" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D456" s="11"/>
       <c r="E456" s="11"/>
@@ -6974,7 +6971,7 @@
       <c r="A457" s="11"/>
       <c r="B457" s="11"/>
       <c r="C457" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D457" s="11"/>
       <c r="E457" s="11"/>
@@ -6983,7 +6980,7 @@
       <c r="A458" s="11"/>
       <c r="B458" s="11"/>
       <c r="C458" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D458" s="11"/>
       <c r="E458" s="11"/>
@@ -6992,7 +6989,7 @@
       <c r="A459" s="11"/>
       <c r="B459" s="11"/>
       <c r="C459" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D459" s="11"/>
       <c r="E459" s="11"/>
@@ -7001,7 +6998,7 @@
       <c r="A460" s="11"/>
       <c r="B460" s="11"/>
       <c r="C460" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D460" s="11"/>
       <c r="E460" s="11"/>
@@ -7010,7 +7007,7 @@
       <c r="A461" s="11"/>
       <c r="B461" s="11"/>
       <c r="C461" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D461" s="11"/>
       <c r="E461" s="11"/>
@@ -7019,7 +7016,7 @@
       <c r="A462" s="11"/>
       <c r="B462" s="11"/>
       <c r="C462" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D462" s="11"/>
       <c r="E462" s="11"/>
@@ -7028,7 +7025,7 @@
       <c r="A463" s="11"/>
       <c r="B463" s="11"/>
       <c r="C463" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D463" s="11"/>
       <c r="E463" s="11"/>
@@ -7037,7 +7034,7 @@
       <c r="A464" s="11"/>
       <c r="B464" s="11"/>
       <c r="C464" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D464" s="11"/>
       <c r="E464" s="11"/>
@@ -7046,7 +7043,7 @@
       <c r="A465" s="11"/>
       <c r="B465" s="11"/>
       <c r="C465" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D465" s="11"/>
       <c r="E465" s="11"/>
@@ -7055,7 +7052,7 @@
       <c r="A466" s="11"/>
       <c r="B466" s="11"/>
       <c r="C466" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D466" s="11"/>
       <c r="E466" s="11"/>
@@ -7065,16 +7062,16 @@
         <v>108.0</v>
       </c>
       <c r="B467" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C467" s="20" t="s">
         <v>406</v>
-      </c>
-      <c r="C467" s="20" t="s">
-        <v>407</v>
       </c>
       <c r="D467" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E467" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="468">
@@ -7082,16 +7079,16 @@
         <v>109.0</v>
       </c>
       <c r="B468" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C468" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="C468" s="8" t="s">
+      <c r="D468" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D468" s="9" t="s">
-        <v>411</v>
-      </c>
       <c r="E468" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="469">
@@ -7099,10 +7096,10 @@
         <v>110.0</v>
       </c>
       <c r="B469" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C469" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C469" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D469" s="9" t="s">
         <v>26</v>
@@ -7140,7 +7137,7 @@
       <c r="A473" s="11"/>
       <c r="B473" s="11"/>
       <c r="C473" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D473" s="11"/>
       <c r="E473" s="11"/>
@@ -7150,13 +7147,13 @@
         <v>111.0</v>
       </c>
       <c r="B474" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C474" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="C474" s="13" t="s">
-        <v>416</v>
-      </c>
       <c r="D474" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E474" s="10" t="s">
         <v>33</v>
@@ -7166,7 +7163,7 @@
       <c r="A475" s="12"/>
       <c r="B475" s="12"/>
       <c r="C475" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D475" s="11"/>
       <c r="E475" s="12"/>
@@ -7176,21 +7173,21 @@
         <v>112.0</v>
       </c>
       <c r="B476" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="C476" s="9" t="s">
         <v>418</v>
-      </c>
-      <c r="C476" s="9" t="s">
-        <v>419</v>
       </c>
       <c r="D476" s="11"/>
       <c r="E476" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="477" ht="35.25" customHeight="1">
       <c r="A477" s="12"/>
       <c r="B477" s="19"/>
       <c r="C477" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D477" s="11"/>
       <c r="E477" s="12"/>
@@ -7200,13 +7197,13 @@
         <v>113.0</v>
       </c>
       <c r="B478" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="C478" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="C478" s="9" t="s">
+      <c r="D478" s="15" t="s">
         <v>422</v>
-      </c>
-      <c r="D478" s="15" t="s">
-        <v>423</v>
       </c>
       <c r="E478" s="10" t="s">
         <v>33</v>
@@ -7216,7 +7213,7 @@
       <c r="A479" s="12"/>
       <c r="B479" s="19"/>
       <c r="C479" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D479" s="21"/>
       <c r="E479" s="11"/>
@@ -7226,13 +7223,13 @@
         <v>114.0</v>
       </c>
       <c r="B480" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C480" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C480" s="9" t="s">
-        <v>426</v>
-      </c>
       <c r="D480" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E480" s="11"/>
     </row>
@@ -7240,14 +7237,14 @@
       <c r="A481" s="12"/>
       <c r="B481" s="19"/>
       <c r="C481" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D481" s="21"/>
       <c r="E481" s="12"/>
     </row>
     <row r="482" ht="23.25" customHeight="1">
       <c r="A482" s="70" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B482" s="4"/>
       <c r="C482" s="4"/>
@@ -7259,13 +7256,13 @@
         <v>115.0</v>
       </c>
       <c r="B483" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C483" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C483" s="9" t="s">
+      <c r="D483" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="D483" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="E483" s="10" t="s">
         <v>44</v>
@@ -7275,7 +7272,7 @@
       <c r="A484" s="12"/>
       <c r="B484" s="12"/>
       <c r="C484" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D484" s="12"/>
       <c r="E484" s="11"/>
@@ -7285,13 +7282,13 @@
         <v>116.0</v>
       </c>
       <c r="B485" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C485" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D485" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E485" s="11"/>
     </row>
@@ -7299,7 +7296,7 @@
       <c r="A486" s="11"/>
       <c r="B486" s="16"/>
       <c r="C486" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D486" s="18"/>
       <c r="E486" s="12"/>
@@ -7309,16 +7306,16 @@
         <v>117.0</v>
       </c>
       <c r="B487" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C487" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="C487" s="9" t="s">
+      <c r="D487" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E487" s="6" t="s">
         <v>430</v>
-      </c>
-      <c r="D487" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="E487" s="6" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="488">
@@ -7326,16 +7323,16 @@
         <v>118.0</v>
       </c>
       <c r="B488" s="71" t="s">
+        <v>431</v>
+      </c>
+      <c r="C488" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C488" s="9" t="s">
+      <c r="D488" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="E488" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="D488" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="E488" s="6" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="489">
@@ -7343,7 +7340,7 @@
         <v>119.0</v>
       </c>
       <c r="B489" s="65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C489" s="9" t="s">
         <v>27</v>
@@ -7352,7 +7349,7 @@
         <v>62</v>
       </c>
       <c r="E489" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="490">
@@ -7378,16 +7375,16 @@
         <v>120.0</v>
       </c>
       <c r="B492" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C492" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C492" s="13" t="s">
-        <v>362</v>
-      </c>
       <c r="D492" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E492" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="493">
@@ -7395,23 +7392,23 @@
         <v>121.0</v>
       </c>
       <c r="B493" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C493" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D493" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E493" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" s="11"/>
       <c r="B494" s="11"/>
       <c r="C494" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D494" s="11"/>
       <c r="E494" s="11"/>
@@ -7420,7 +7417,7 @@
       <c r="A495" s="11"/>
       <c r="B495" s="11"/>
       <c r="C495" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D495" s="11"/>
       <c r="E495" s="11"/>
@@ -7429,7 +7426,7 @@
       <c r="A496" s="11"/>
       <c r="B496" s="11"/>
       <c r="C496" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D496" s="11"/>
       <c r="E496" s="11"/>
@@ -7438,7 +7435,7 @@
       <c r="A497" s="11"/>
       <c r="B497" s="11"/>
       <c r="C497" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D497" s="11"/>
       <c r="E497" s="11"/>
@@ -7447,7 +7444,7 @@
       <c r="A498" s="11"/>
       <c r="B498" s="11"/>
       <c r="C498" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D498" s="11"/>
       <c r="E498" s="11"/>
@@ -7456,7 +7453,7 @@
       <c r="A499" s="11"/>
       <c r="B499" s="11"/>
       <c r="C499" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D499" s="11"/>
       <c r="E499" s="11"/>
@@ -7465,7 +7462,7 @@
       <c r="A500" s="11"/>
       <c r="B500" s="11"/>
       <c r="C500" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D500" s="11"/>
       <c r="E500" s="11"/>
@@ -7474,7 +7471,7 @@
       <c r="A501" s="11"/>
       <c r="B501" s="11"/>
       <c r="C501" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D501" s="11"/>
       <c r="E501" s="11"/>
@@ -7483,7 +7480,7 @@
       <c r="A502" s="11"/>
       <c r="B502" s="11"/>
       <c r="C502" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D502" s="11"/>
       <c r="E502" s="11"/>
@@ -7492,7 +7489,7 @@
       <c r="A503" s="11"/>
       <c r="B503" s="11"/>
       <c r="C503" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D503" s="11"/>
       <c r="E503" s="11"/>
@@ -7501,7 +7498,7 @@
       <c r="A504" s="11"/>
       <c r="B504" s="11"/>
       <c r="C504" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D504" s="11"/>
       <c r="E504" s="11"/>
@@ -7510,7 +7507,7 @@
       <c r="A505" s="11"/>
       <c r="B505" s="11"/>
       <c r="C505" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D505" s="11"/>
       <c r="E505" s="11"/>
@@ -7519,7 +7516,7 @@
       <c r="A506" s="11"/>
       <c r="B506" s="11"/>
       <c r="C506" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D506" s="11"/>
       <c r="E506" s="11"/>
@@ -7528,7 +7525,7 @@
       <c r="A507" s="11"/>
       <c r="B507" s="11"/>
       <c r="C507" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D507" s="11"/>
       <c r="E507" s="11"/>
@@ -7537,7 +7534,7 @@
       <c r="A508" s="11"/>
       <c r="B508" s="11"/>
       <c r="C508" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D508" s="11"/>
       <c r="E508" s="11"/>
@@ -7546,7 +7543,7 @@
       <c r="A509" s="11"/>
       <c r="B509" s="11"/>
       <c r="C509" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D509" s="11"/>
       <c r="E509" s="11"/>
@@ -7555,7 +7552,7 @@
       <c r="A510" s="11"/>
       <c r="B510" s="11"/>
       <c r="C510" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D510" s="11"/>
       <c r="E510" s="11"/>
@@ -7564,7 +7561,7 @@
       <c r="A511" s="11"/>
       <c r="B511" s="11"/>
       <c r="C511" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D511" s="11"/>
       <c r="E511" s="11"/>
@@ -7573,7 +7570,7 @@
       <c r="A512" s="11"/>
       <c r="B512" s="11"/>
       <c r="C512" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D512" s="11"/>
       <c r="E512" s="11"/>
@@ -7582,7 +7579,7 @@
       <c r="A513" s="11"/>
       <c r="B513" s="11"/>
       <c r="C513" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D513" s="11"/>
       <c r="E513" s="11"/>
@@ -7591,7 +7588,7 @@
       <c r="A514" s="11"/>
       <c r="B514" s="11"/>
       <c r="C514" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D514" s="11"/>
       <c r="E514" s="11"/>
@@ -7600,7 +7597,7 @@
       <c r="A515" s="11"/>
       <c r="B515" s="11"/>
       <c r="C515" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D515" s="11"/>
       <c r="E515" s="11"/>
@@ -7609,7 +7606,7 @@
       <c r="A516" s="11"/>
       <c r="B516" s="11"/>
       <c r="C516" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D516" s="11"/>
       <c r="E516" s="11"/>
@@ -7618,7 +7615,7 @@
       <c r="A517" s="11"/>
       <c r="B517" s="11"/>
       <c r="C517" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D517" s="11"/>
       <c r="E517" s="11"/>
@@ -7627,7 +7624,7 @@
       <c r="A518" s="11"/>
       <c r="B518" s="11"/>
       <c r="C518" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D518" s="11"/>
       <c r="E518" s="11"/>
@@ -7636,7 +7633,7 @@
       <c r="A519" s="11"/>
       <c r="B519" s="11"/>
       <c r="C519" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D519" s="11"/>
       <c r="E519" s="11"/>
@@ -7645,7 +7642,7 @@
       <c r="A520" s="11"/>
       <c r="B520" s="11"/>
       <c r="C520" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D520" s="11"/>
       <c r="E520" s="11"/>
@@ -7654,7 +7651,7 @@
       <c r="A521" s="11"/>
       <c r="B521" s="11"/>
       <c r="C521" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D521" s="11"/>
       <c r="E521" s="11"/>
@@ -7663,7 +7660,7 @@
       <c r="A522" s="11"/>
       <c r="B522" s="11"/>
       <c r="C522" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D522" s="11"/>
       <c r="E522" s="11"/>
@@ -7672,7 +7669,7 @@
       <c r="A523" s="11"/>
       <c r="B523" s="11"/>
       <c r="C523" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D523" s="11"/>
       <c r="E523" s="11"/>
@@ -7681,7 +7678,7 @@
       <c r="A524" s="11"/>
       <c r="B524" s="11"/>
       <c r="C524" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D524" s="11"/>
       <c r="E524" s="11"/>
@@ -7690,7 +7687,7 @@
       <c r="A525" s="11"/>
       <c r="B525" s="11"/>
       <c r="C525" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D525" s="11"/>
       <c r="E525" s="11"/>
@@ -7699,7 +7696,7 @@
       <c r="A526" s="11"/>
       <c r="B526" s="11"/>
       <c r="C526" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D526" s="11"/>
       <c r="E526" s="11"/>
@@ -7708,7 +7705,7 @@
       <c r="A527" s="11"/>
       <c r="B527" s="11"/>
       <c r="C527" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D527" s="11"/>
       <c r="E527" s="11"/>
@@ -7717,7 +7714,7 @@
       <c r="A528" s="11"/>
       <c r="B528" s="11"/>
       <c r="C528" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D528" s="11"/>
       <c r="E528" s="11"/>
@@ -7726,7 +7723,7 @@
       <c r="A529" s="11"/>
       <c r="B529" s="11"/>
       <c r="C529" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D529" s="11"/>
       <c r="E529" s="11"/>
@@ -7735,7 +7732,7 @@
       <c r="A530" s="11"/>
       <c r="B530" s="11"/>
       <c r="C530" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D530" s="11"/>
       <c r="E530" s="11"/>
@@ -7744,7 +7741,7 @@
       <c r="A531" s="11"/>
       <c r="B531" s="11"/>
       <c r="C531" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D531" s="11"/>
       <c r="E531" s="11"/>
@@ -7753,7 +7750,7 @@
       <c r="A532" s="11"/>
       <c r="B532" s="11"/>
       <c r="C532" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D532" s="11"/>
       <c r="E532" s="11"/>
@@ -7762,7 +7759,7 @@
       <c r="A533" s="11"/>
       <c r="B533" s="11"/>
       <c r="C533" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D533" s="11"/>
       <c r="E533" s="11"/>
@@ -7772,16 +7769,16 @@
         <v>122.0</v>
       </c>
       <c r="B534" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C534" s="64" t="s">
         <v>406</v>
-      </c>
-      <c r="C534" s="64" t="s">
-        <v>407</v>
       </c>
       <c r="D534" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E534" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="535">
@@ -7789,16 +7786,16 @@
         <v>123.0</v>
       </c>
       <c r="B535" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C535" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D535" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E535" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="536">
@@ -7806,10 +7803,10 @@
         <v>124.0</v>
       </c>
       <c r="B536" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C536" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C536" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D536" s="9" t="s">
         <v>26</v>
@@ -7847,7 +7844,7 @@
       <c r="A540" s="11"/>
       <c r="B540" s="11"/>
       <c r="C540" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D540" s="11"/>
       <c r="E540" s="11"/>
@@ -7857,13 +7854,13 @@
         <v>125.0</v>
       </c>
       <c r="B541" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C541" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D541" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E541" s="10" t="s">
         <v>44</v>
@@ -7873,7 +7870,7 @@
       <c r="A542" s="11"/>
       <c r="B542" s="11"/>
       <c r="C542" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D542" s="11"/>
       <c r="E542" s="11"/>
@@ -7883,13 +7880,13 @@
         <v>126.0</v>
       </c>
       <c r="B543" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C543" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C543" s="9" t="s">
-        <v>426</v>
-      </c>
       <c r="D543" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E543" s="11"/>
     </row>
@@ -7897,14 +7894,14 @@
       <c r="A544" s="12"/>
       <c r="B544" s="12"/>
       <c r="C544" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D544" s="12"/>
       <c r="E544" s="12"/>
     </row>
     <row r="545" ht="22.5" customHeight="1">
       <c r="A545" s="70" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B545" s="4"/>
       <c r="C545" s="4"/>
@@ -7916,13 +7913,13 @@
         <v>127.0</v>
       </c>
       <c r="B546" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C546" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D546" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E546" s="10" t="s">
         <v>54</v>
@@ -7933,7 +7930,7 @@
         <v>128.0</v>
       </c>
       <c r="B547" s="65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C547" s="17" t="s">
         <v>27</v>
@@ -7966,16 +7963,16 @@
         <v>129.0</v>
       </c>
       <c r="B550" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C550" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C550" s="13" t="s">
-        <v>362</v>
-      </c>
       <c r="D550" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E550" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="551">
@@ -7983,23 +7980,23 @@
         <v>130.0</v>
       </c>
       <c r="B551" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C551" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D551" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E551" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" s="11"/>
       <c r="B552" s="11"/>
       <c r="C552" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D552" s="11"/>
       <c r="E552" s="11"/>
@@ -8008,7 +8005,7 @@
       <c r="A553" s="11"/>
       <c r="B553" s="11"/>
       <c r="C553" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D553" s="11"/>
       <c r="E553" s="11"/>
@@ -8017,7 +8014,7 @@
       <c r="A554" s="11"/>
       <c r="B554" s="11"/>
       <c r="C554" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D554" s="11"/>
       <c r="E554" s="11"/>
@@ -8026,7 +8023,7 @@
       <c r="A555" s="11"/>
       <c r="B555" s="11"/>
       <c r="C555" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D555" s="11"/>
       <c r="E555" s="11"/>
@@ -8035,7 +8032,7 @@
       <c r="A556" s="11"/>
       <c r="B556" s="11"/>
       <c r="C556" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D556" s="11"/>
       <c r="E556" s="11"/>
@@ -8044,7 +8041,7 @@
       <c r="A557" s="11"/>
       <c r="B557" s="11"/>
       <c r="C557" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D557" s="11"/>
       <c r="E557" s="11"/>
@@ -8053,7 +8050,7 @@
       <c r="A558" s="11"/>
       <c r="B558" s="11"/>
       <c r="C558" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D558" s="11"/>
       <c r="E558" s="11"/>
@@ -8062,7 +8059,7 @@
       <c r="A559" s="11"/>
       <c r="B559" s="11"/>
       <c r="C559" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D559" s="11"/>
       <c r="E559" s="11"/>
@@ -8071,7 +8068,7 @@
       <c r="A560" s="11"/>
       <c r="B560" s="11"/>
       <c r="C560" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D560" s="11"/>
       <c r="E560" s="11"/>
@@ -8080,7 +8077,7 @@
       <c r="A561" s="11"/>
       <c r="B561" s="11"/>
       <c r="C561" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D561" s="11"/>
       <c r="E561" s="11"/>
@@ -8089,7 +8086,7 @@
       <c r="A562" s="11"/>
       <c r="B562" s="11"/>
       <c r="C562" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D562" s="11"/>
       <c r="E562" s="11"/>
@@ -8098,7 +8095,7 @@
       <c r="A563" s="11"/>
       <c r="B563" s="11"/>
       <c r="C563" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D563" s="11"/>
       <c r="E563" s="11"/>
@@ -8107,7 +8104,7 @@
       <c r="A564" s="11"/>
       <c r="B564" s="11"/>
       <c r="C564" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D564" s="11"/>
       <c r="E564" s="11"/>
@@ -8116,7 +8113,7 @@
       <c r="A565" s="11"/>
       <c r="B565" s="11"/>
       <c r="C565" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D565" s="11"/>
       <c r="E565" s="11"/>
@@ -8125,7 +8122,7 @@
       <c r="A566" s="11"/>
       <c r="B566" s="11"/>
       <c r="C566" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D566" s="11"/>
       <c r="E566" s="11"/>
@@ -8134,7 +8131,7 @@
       <c r="A567" s="11"/>
       <c r="B567" s="11"/>
       <c r="C567" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D567" s="11"/>
       <c r="E567" s="11"/>
@@ -8143,7 +8140,7 @@
       <c r="A568" s="11"/>
       <c r="B568" s="11"/>
       <c r="C568" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D568" s="11"/>
       <c r="E568" s="11"/>
@@ -8152,7 +8149,7 @@
       <c r="A569" s="11"/>
       <c r="B569" s="11"/>
       <c r="C569" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D569" s="11"/>
       <c r="E569" s="11"/>
@@ -8161,7 +8158,7 @@
       <c r="A570" s="11"/>
       <c r="B570" s="11"/>
       <c r="C570" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D570" s="11"/>
       <c r="E570" s="11"/>
@@ -8170,7 +8167,7 @@
       <c r="A571" s="11"/>
       <c r="B571" s="11"/>
       <c r="C571" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D571" s="11"/>
       <c r="E571" s="11"/>
@@ -8179,7 +8176,7 @@
       <c r="A572" s="11"/>
       <c r="B572" s="11"/>
       <c r="C572" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D572" s="11"/>
       <c r="E572" s="11"/>
@@ -8188,7 +8185,7 @@
       <c r="A573" s="11"/>
       <c r="B573" s="11"/>
       <c r="C573" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D573" s="11"/>
       <c r="E573" s="11"/>
@@ -8197,7 +8194,7 @@
       <c r="A574" s="11"/>
       <c r="B574" s="11"/>
       <c r="C574" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D574" s="11"/>
       <c r="E574" s="11"/>
@@ -8206,7 +8203,7 @@
       <c r="A575" s="11"/>
       <c r="B575" s="11"/>
       <c r="C575" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D575" s="11"/>
       <c r="E575" s="11"/>
@@ -8215,7 +8212,7 @@
       <c r="A576" s="11"/>
       <c r="B576" s="11"/>
       <c r="C576" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D576" s="11"/>
       <c r="E576" s="11"/>
@@ -8224,7 +8221,7 @@
       <c r="A577" s="11"/>
       <c r="B577" s="11"/>
       <c r="C577" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D577" s="11"/>
       <c r="E577" s="11"/>
@@ -8233,7 +8230,7 @@
       <c r="A578" s="11"/>
       <c r="B578" s="11"/>
       <c r="C578" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D578" s="11"/>
       <c r="E578" s="11"/>
@@ -8242,7 +8239,7 @@
       <c r="A579" s="11"/>
       <c r="B579" s="11"/>
       <c r="C579" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D579" s="11"/>
       <c r="E579" s="11"/>
@@ -8251,7 +8248,7 @@
       <c r="A580" s="11"/>
       <c r="B580" s="11"/>
       <c r="C580" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D580" s="11"/>
       <c r="E580" s="11"/>
@@ -8260,7 +8257,7 @@
       <c r="A581" s="11"/>
       <c r="B581" s="11"/>
       <c r="C581" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D581" s="11"/>
       <c r="E581" s="11"/>
@@ -8269,7 +8266,7 @@
       <c r="A582" s="11"/>
       <c r="B582" s="11"/>
       <c r="C582" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D582" s="11"/>
       <c r="E582" s="11"/>
@@ -8278,7 +8275,7 @@
       <c r="A583" s="11"/>
       <c r="B583" s="11"/>
       <c r="C583" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D583" s="11"/>
       <c r="E583" s="11"/>
@@ -8287,7 +8284,7 @@
       <c r="A584" s="11"/>
       <c r="B584" s="11"/>
       <c r="C584" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D584" s="11"/>
       <c r="E584" s="11"/>
@@ -8296,7 +8293,7 @@
       <c r="A585" s="11"/>
       <c r="B585" s="11"/>
       <c r="C585" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D585" s="11"/>
       <c r="E585" s="11"/>
@@ -8305,7 +8302,7 @@
       <c r="A586" s="11"/>
       <c r="B586" s="11"/>
       <c r="C586" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D586" s="11"/>
       <c r="E586" s="11"/>
@@ -8314,7 +8311,7 @@
       <c r="A587" s="11"/>
       <c r="B587" s="11"/>
       <c r="C587" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D587" s="11"/>
       <c r="E587" s="11"/>
@@ -8323,7 +8320,7 @@
       <c r="A588" s="11"/>
       <c r="B588" s="11"/>
       <c r="C588" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D588" s="11"/>
       <c r="E588" s="11"/>
@@ -8332,7 +8329,7 @@
       <c r="A589" s="11"/>
       <c r="B589" s="11"/>
       <c r="C589" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D589" s="11"/>
       <c r="E589" s="11"/>
@@ -8341,7 +8338,7 @@
       <c r="A590" s="11"/>
       <c r="B590" s="11"/>
       <c r="C590" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D590" s="11"/>
       <c r="E590" s="11"/>
@@ -8350,7 +8347,7 @@
       <c r="A591" s="11"/>
       <c r="B591" s="11"/>
       <c r="C591" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D591" s="11"/>
       <c r="E591" s="11"/>
@@ -8360,16 +8357,16 @@
         <v>131.0</v>
       </c>
       <c r="B592" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C592" s="64" t="s">
         <v>406</v>
-      </c>
-      <c r="C592" s="64" t="s">
-        <v>407</v>
       </c>
       <c r="D592" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E592" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="593">
@@ -8377,16 +8374,16 @@
         <v>132.0</v>
       </c>
       <c r="B593" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D593" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E593" s="72" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="594">
@@ -8394,10 +8391,10 @@
         <v>133.0</v>
       </c>
       <c r="B594" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C594" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C594" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D594" s="9" t="s">
         <v>26</v>
@@ -8435,7 +8432,7 @@
       <c r="A598" s="11"/>
       <c r="B598" s="11"/>
       <c r="C598" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D598" s="11"/>
       <c r="E598" s="11"/>
@@ -8445,13 +8442,13 @@
         <v>134.0</v>
       </c>
       <c r="B599" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C599" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D599" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E599" s="72" t="s">
         <v>54</v>
@@ -8461,7 +8458,7 @@
       <c r="A600" s="11"/>
       <c r="B600" s="11"/>
       <c r="C600" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D600" s="11"/>
       <c r="E600" s="11"/>
@@ -8471,13 +8468,13 @@
         <v>135.0</v>
       </c>
       <c r="B601" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C601" s="73" t="s">
         <v>425</v>
       </c>
-      <c r="C601" s="73" t="s">
-        <v>426</v>
-      </c>
       <c r="D601" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E601" s="11"/>
     </row>
@@ -8485,7 +8482,7 @@
       <c r="A602" s="12"/>
       <c r="B602" s="19"/>
       <c r="C602" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D602" s="21"/>
       <c r="E602" s="12"/>

</xml_diff>

<commit_message>
CLDC-2372 Update bulk upload resources (#1671)
* Reorder resources list

* Update sales 23/24 resources

* Update sales 22/23 resources

* Fix typo and add missing paths

* Change the wording

* feat: update files, add 22/23 lettings form to local storage and add collection resources helper

* feat: remove sales bu feature toggoe

* refactor: lint

* refactor: erblinting

* feat: add tests for helper

* feat: revert feature flag removal (will put in a separate PR)

* refactor: update matadata helper

---------

Co-authored-by: natdeanlewissoftwire <nat.dean-lewis@softwire.com>
</commit_message>
<xml_diff>
--- a/public/files/bulk-upload-sales-specification-2023-24.xlsx
+++ b/public/files/bulk-upload-sales-specification-2023-24.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="444">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="974" uniqueCount="443">
   <si>
     <t>Field number</t>
   </si>
@@ -398,9 +398,6 @@
   </si>
   <si>
     <t>Numeric, range 1 only</t>
-  </si>
-  <si>
-    <t>Yes, if buyer was not interviewed (if field 28 = 1)</t>
   </si>
   <si>
     <t>What is buyer 1’s age?</t>
@@ -3026,7 +3023,7 @@
         <v>118</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
     </row>
     <row r="77">
@@ -3052,16 +3049,16 @@
         <v>30.0</v>
       </c>
       <c r="B79" s="20" t="s">
+        <v>119</v>
+      </c>
+      <c r="C79" s="20" t="s">
         <v>120</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="D79" s="20" t="s">
         <v>121</v>
       </c>
-      <c r="D79" s="20" t="s">
+      <c r="E79" s="26" t="s">
         <v>122</v>
-      </c>
-      <c r="E79" s="26" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="80">
@@ -3069,23 +3066,23 @@
         <v>31.0</v>
       </c>
       <c r="B80" s="17" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C80" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D80" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" s="11"/>
       <c r="B81" s="11"/>
       <c r="C81" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E81" s="11"/>
     </row>
@@ -3093,7 +3090,7 @@
       <c r="A82" s="11"/>
       <c r="B82" s="11"/>
       <c r="C82" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E82" s="11"/>
     </row>
@@ -3101,7 +3098,7 @@
       <c r="A83" s="11"/>
       <c r="B83" s="11"/>
       <c r="C83" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E83" s="11"/>
     </row>
@@ -3109,7 +3106,7 @@
       <c r="A84" s="12"/>
       <c r="B84" s="12"/>
       <c r="C84" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D84" s="35"/>
       <c r="E84" s="12"/>
@@ -3119,23 +3116,23 @@
         <v>32.0</v>
       </c>
       <c r="B85" s="17" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C85" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D85" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="11"/>
       <c r="B86" s="11"/>
       <c r="C86" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D86" s="11"/>
       <c r="E86" s="11"/>
@@ -3144,7 +3141,7 @@
       <c r="A87" s="11"/>
       <c r="B87" s="11"/>
       <c r="C87" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D87" s="11"/>
       <c r="E87" s="11"/>
@@ -3153,7 +3150,7 @@
       <c r="A88" s="11"/>
       <c r="B88" s="11"/>
       <c r="C88" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D88" s="11"/>
       <c r="E88" s="11"/>
@@ -3162,7 +3159,7 @@
       <c r="A89" s="11"/>
       <c r="B89" s="11"/>
       <c r="C89" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D89" s="11"/>
       <c r="E89" s="11"/>
@@ -3171,7 +3168,7 @@
       <c r="A90" s="11"/>
       <c r="B90" s="11"/>
       <c r="C90" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D90" s="11"/>
       <c r="E90" s="11"/>
@@ -3180,7 +3177,7 @@
       <c r="A91" s="11"/>
       <c r="B91" s="11"/>
       <c r="C91" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D91" s="11"/>
       <c r="E91" s="11"/>
@@ -3189,7 +3186,7 @@
       <c r="A92" s="11"/>
       <c r="B92" s="11"/>
       <c r="C92" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D92" s="11"/>
       <c r="E92" s="11"/>
@@ -3198,7 +3195,7 @@
       <c r="A93" s="11"/>
       <c r="B93" s="11"/>
       <c r="C93" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D93" s="11"/>
       <c r="E93" s="11"/>
@@ -3207,7 +3204,7 @@
       <c r="A94" s="11"/>
       <c r="B94" s="11"/>
       <c r="C94" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D94" s="11"/>
       <c r="E94" s="11"/>
@@ -3216,7 +3213,7 @@
       <c r="A95" s="11"/>
       <c r="B95" s="11"/>
       <c r="C95" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D95" s="11"/>
       <c r="E95" s="11"/>
@@ -3225,7 +3222,7 @@
       <c r="A96" s="11"/>
       <c r="B96" s="11"/>
       <c r="C96" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D96" s="11"/>
       <c r="E96" s="11"/>
@@ -3234,7 +3231,7 @@
       <c r="A97" s="11"/>
       <c r="B97" s="11"/>
       <c r="C97" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D97" s="11"/>
       <c r="E97" s="11"/>
@@ -3243,7 +3240,7 @@
       <c r="A98" s="11"/>
       <c r="B98" s="11"/>
       <c r="C98" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D98" s="11"/>
       <c r="E98" s="11"/>
@@ -3252,7 +3249,7 @@
       <c r="A99" s="11"/>
       <c r="B99" s="11"/>
       <c r="C99" s="17" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D99" s="11"/>
       <c r="E99" s="11"/>
@@ -3261,7 +3258,7 @@
       <c r="A100" s="11"/>
       <c r="B100" s="11"/>
       <c r="C100" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D100" s="11"/>
       <c r="E100" s="11"/>
@@ -3270,7 +3267,7 @@
       <c r="A101" s="11"/>
       <c r="B101" s="11"/>
       <c r="C101" s="32" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="D101" s="11"/>
       <c r="E101" s="11"/>
@@ -3279,7 +3276,7 @@
       <c r="A102" s="11"/>
       <c r="B102" s="11"/>
       <c r="C102" s="37" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="D102" s="11"/>
       <c r="E102" s="11"/>
@@ -3288,7 +3285,7 @@
       <c r="A103" s="11"/>
       <c r="B103" s="11"/>
       <c r="C103" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D103" s="11"/>
       <c r="E103" s="11"/>
@@ -3297,7 +3294,7 @@
       <c r="A104" s="12"/>
       <c r="B104" s="12"/>
       <c r="C104" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -3307,23 +3304,23 @@
         <v>33.0</v>
       </c>
       <c r="B105" s="17" t="s">
+        <v>150</v>
+      </c>
+      <c r="C105" s="13" t="s">
         <v>151</v>
       </c>
-      <c r="C105" s="13" t="s">
+      <c r="D105" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D105" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E105" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="106">
       <c r="A106" s="11"/>
       <c r="B106" s="11"/>
       <c r="C106" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D106" s="11"/>
       <c r="E106" s="11"/>
@@ -3332,7 +3329,7 @@
       <c r="A107" s="11"/>
       <c r="B107" s="11"/>
       <c r="C107" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D107" s="11"/>
       <c r="E107" s="11"/>
@@ -3341,7 +3338,7 @@
       <c r="A108" s="11"/>
       <c r="B108" s="11"/>
       <c r="C108" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D108" s="11"/>
       <c r="E108" s="11"/>
@@ -3350,7 +3347,7 @@
       <c r="A109" s="11"/>
       <c r="B109" s="11"/>
       <c r="C109" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D109" s="11"/>
       <c r="E109" s="11"/>
@@ -3359,7 +3356,7 @@
       <c r="A110" s="12"/>
       <c r="B110" s="12"/>
       <c r="C110" s="39" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -3369,16 +3366,16 @@
         <v>34.0</v>
       </c>
       <c r="B111" s="20" t="s">
+        <v>158</v>
+      </c>
+      <c r="C111" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="C111" s="7" t="s">
-        <v>160</v>
       </c>
       <c r="D111" s="20" t="s">
         <v>97</v>
       </c>
       <c r="E111" s="26" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="112">
@@ -3386,23 +3383,23 @@
         <v>35.0</v>
       </c>
       <c r="B112" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C112" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D112" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="113">
       <c r="A113" s="11"/>
       <c r="B113" s="11"/>
       <c r="C113" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D113" s="11"/>
       <c r="E113" s="11"/>
@@ -3411,7 +3408,7 @@
       <c r="A114" s="11"/>
       <c r="B114" s="11"/>
       <c r="C114" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D114" s="11"/>
       <c r="E114" s="11"/>
@@ -3420,7 +3417,7 @@
       <c r="A115" s="11"/>
       <c r="B115" s="11"/>
       <c r="C115" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D115" s="11"/>
       <c r="E115" s="11"/>
@@ -3429,7 +3426,7 @@
       <c r="A116" s="11"/>
       <c r="B116" s="11"/>
       <c r="C116" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D116" s="11"/>
       <c r="E116" s="11"/>
@@ -3438,7 +3435,7 @@
       <c r="A117" s="11"/>
       <c r="B117" s="11"/>
       <c r="C117" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D117" s="11"/>
       <c r="E117" s="11"/>
@@ -3447,7 +3444,7 @@
       <c r="A118" s="11"/>
       <c r="B118" s="11"/>
       <c r="C118" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D118" s="11"/>
       <c r="E118" s="11"/>
@@ -3456,7 +3453,7 @@
       <c r="A119" s="11"/>
       <c r="B119" s="11"/>
       <c r="C119" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D119" s="11"/>
       <c r="E119" s="11"/>
@@ -3465,7 +3462,7 @@
       <c r="A120" s="11"/>
       <c r="B120" s="11"/>
       <c r="C120" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D120" s="11"/>
       <c r="E120" s="11"/>
@@ -3474,7 +3471,7 @@
       <c r="A121" s="11"/>
       <c r="B121" s="11"/>
       <c r="C121" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D121" s="11"/>
       <c r="E121" s="11"/>
@@ -3483,7 +3480,7 @@
       <c r="A122" s="12"/>
       <c r="B122" s="12"/>
       <c r="C122" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D122" s="12"/>
       <c r="E122" s="12"/>
@@ -3493,7 +3490,7 @@
         <v>36.0</v>
       </c>
       <c r="B123" s="9" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="C123" s="17" t="s">
         <v>27</v>
@@ -3502,7 +3499,7 @@
         <v>62</v>
       </c>
       <c r="E123" s="10" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="124">
@@ -3528,23 +3525,23 @@
         <v>37.0</v>
       </c>
       <c r="B126" s="17" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="C126" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D126" s="17" t="s">
+        <v>175</v>
+      </c>
+      <c r="E126" s="40" t="s">
         <v>176</v>
-      </c>
-      <c r="E126" s="40" t="s">
-        <v>177</v>
       </c>
     </row>
     <row r="127">
       <c r="A127" s="11"/>
       <c r="B127" s="11"/>
       <c r="C127" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D127" s="11"/>
       <c r="E127" s="11"/>
@@ -3553,7 +3550,7 @@
       <c r="A128" s="11"/>
       <c r="B128" s="11"/>
       <c r="C128" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D128" s="11"/>
       <c r="E128" s="11"/>
@@ -3562,7 +3559,7 @@
       <c r="A129" s="11"/>
       <c r="B129" s="11"/>
       <c r="C129" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D129" s="11"/>
       <c r="E129" s="11"/>
@@ -3571,7 +3568,7 @@
       <c r="A130" s="12"/>
       <c r="B130" s="12"/>
       <c r="C130" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D130" s="12"/>
       <c r="E130" s="12"/>
@@ -3581,16 +3578,16 @@
         <v>38.0</v>
       </c>
       <c r="B131" s="8" t="s">
+        <v>180</v>
+      </c>
+      <c r="C131" s="20" t="s">
         <v>181</v>
       </c>
-      <c r="C131" s="20" t="s">
+      <c r="D131" s="20" t="s">
         <v>182</v>
       </c>
-      <c r="D131" s="20" t="s">
+      <c r="E131" s="26" t="s">
         <v>183</v>
-      </c>
-      <c r="E131" s="26" t="s">
-        <v>184</v>
       </c>
     </row>
     <row r="132">
@@ -3598,23 +3595,23 @@
         <v>39.0</v>
       </c>
       <c r="B132" s="17" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C132" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D132" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E132" s="41" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="133">
       <c r="A133" s="11"/>
       <c r="B133" s="11"/>
       <c r="C133" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E133" s="11"/>
     </row>
@@ -3622,7 +3619,7 @@
       <c r="A134" s="11"/>
       <c r="B134" s="11"/>
       <c r="C134" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E134" s="11"/>
     </row>
@@ -3630,7 +3627,7 @@
       <c r="A135" s="11"/>
       <c r="B135" s="11"/>
       <c r="C135" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E135" s="11"/>
     </row>
@@ -3638,7 +3635,7 @@
       <c r="A136" s="12"/>
       <c r="B136" s="12"/>
       <c r="C136" s="20" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="D136" s="35"/>
       <c r="E136" s="12"/>
@@ -3648,23 +3645,23 @@
         <v>40.0</v>
       </c>
       <c r="B137" s="17" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C137" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D137" s="17" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="E137" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="138">
       <c r="A138" s="11"/>
       <c r="B138" s="11"/>
       <c r="C138" s="32" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D138" s="11"/>
       <c r="E138" s="11"/>
@@ -3673,7 +3670,7 @@
       <c r="A139" s="11"/>
       <c r="B139" s="11"/>
       <c r="C139" s="32" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="D139" s="11"/>
       <c r="E139" s="11"/>
@@ -3682,7 +3679,7 @@
       <c r="A140" s="11"/>
       <c r="B140" s="11"/>
       <c r="C140" s="32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="D140" s="11"/>
       <c r="E140" s="11"/>
@@ -3691,7 +3688,7 @@
       <c r="A141" s="11"/>
       <c r="B141" s="11"/>
       <c r="C141" s="32" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="D141" s="11"/>
       <c r="E141" s="11"/>
@@ -3700,7 +3697,7 @@
       <c r="A142" s="11"/>
       <c r="B142" s="11"/>
       <c r="C142" s="32" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D142" s="11"/>
       <c r="E142" s="11"/>
@@ -3709,7 +3706,7 @@
       <c r="A143" s="11"/>
       <c r="B143" s="11"/>
       <c r="C143" s="32" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D143" s="11"/>
       <c r="E143" s="11"/>
@@ -3718,7 +3715,7 @@
       <c r="A144" s="11"/>
       <c r="B144" s="11"/>
       <c r="C144" s="32" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D144" s="11"/>
       <c r="E144" s="11"/>
@@ -3727,7 +3724,7 @@
       <c r="A145" s="11"/>
       <c r="B145" s="11"/>
       <c r="C145" s="17" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="D145" s="11"/>
       <c r="E145" s="11"/>
@@ -3736,7 +3733,7 @@
       <c r="A146" s="11"/>
       <c r="B146" s="11"/>
       <c r="C146" s="32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D146" s="11"/>
       <c r="E146" s="11"/>
@@ -3745,7 +3742,7 @@
       <c r="A147" s="11"/>
       <c r="B147" s="11"/>
       <c r="C147" s="32" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D147" s="11"/>
       <c r="E147" s="11"/>
@@ -3754,7 +3751,7 @@
       <c r="A148" s="11"/>
       <c r="B148" s="11"/>
       <c r="C148" s="32" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="D148" s="11"/>
       <c r="E148" s="11"/>
@@ -3763,7 +3760,7 @@
       <c r="A149" s="11"/>
       <c r="B149" s="11"/>
       <c r="C149" s="32" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D149" s="11"/>
       <c r="E149" s="11"/>
@@ -3772,7 +3769,7 @@
       <c r="A150" s="11"/>
       <c r="B150" s="11"/>
       <c r="C150" s="32" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D150" s="11"/>
       <c r="E150" s="11"/>
@@ -3781,7 +3778,7 @@
       <c r="A151" s="11"/>
       <c r="B151" s="11"/>
       <c r="C151" s="17" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="D151" s="11"/>
       <c r="E151" s="11"/>
@@ -3790,7 +3787,7 @@
       <c r="A152" s="11"/>
       <c r="B152" s="11"/>
       <c r="C152" s="32" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="D152" s="11"/>
       <c r="E152" s="11"/>
@@ -3799,7 +3796,7 @@
       <c r="A153" s="11"/>
       <c r="B153" s="11"/>
       <c r="C153" s="32" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="D153" s="11"/>
       <c r="E153" s="11"/>
@@ -3808,7 +3805,7 @@
       <c r="A154" s="11"/>
       <c r="B154" s="11"/>
       <c r="C154" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D154" s="11"/>
       <c r="E154" s="11"/>
@@ -3817,7 +3814,7 @@
       <c r="A155" s="11"/>
       <c r="B155" s="11"/>
       <c r="C155" s="37" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D155" s="11"/>
       <c r="E155" s="11"/>
@@ -3826,7 +3823,7 @@
       <c r="A156" s="12"/>
       <c r="B156" s="12"/>
       <c r="C156" s="38" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D156" s="12"/>
       <c r="E156" s="11"/>
@@ -3836,23 +3833,23 @@
         <v>41.0</v>
       </c>
       <c r="B157" s="17" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="C157" s="13" t="s">
+        <v>151</v>
+      </c>
+      <c r="D157" s="17" t="s">
         <v>152</v>
       </c>
-      <c r="D157" s="17" t="s">
-        <v>153</v>
-      </c>
       <c r="E157" s="40" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="158">
       <c r="A158" s="11"/>
       <c r="B158" s="11"/>
       <c r="C158" s="13" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="D158" s="11"/>
       <c r="E158" s="11"/>
@@ -3861,7 +3858,7 @@
       <c r="A159" s="11"/>
       <c r="B159" s="11"/>
       <c r="C159" s="36" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="D159" s="11"/>
       <c r="E159" s="11"/>
@@ -3870,7 +3867,7 @@
       <c r="A160" s="11"/>
       <c r="B160" s="11"/>
       <c r="C160" s="36" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="D160" s="11"/>
       <c r="E160" s="11"/>
@@ -3879,7 +3876,7 @@
       <c r="A161" s="11"/>
       <c r="B161" s="11"/>
       <c r="C161" s="36" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="D161" s="11"/>
       <c r="E161" s="11"/>
@@ -3888,7 +3885,7 @@
       <c r="A162" s="12"/>
       <c r="B162" s="12"/>
       <c r="C162" s="38" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="D162" s="12"/>
       <c r="E162" s="12"/>
@@ -3898,16 +3895,16 @@
         <v>42.0</v>
       </c>
       <c r="B163" s="20" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C163" s="7" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="D163" s="20" t="s">
         <v>97</v>
       </c>
       <c r="E163" s="26" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="164">
@@ -3915,23 +3912,23 @@
         <v>43.0</v>
       </c>
       <c r="B164" s="17" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C164" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D164" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E164" s="40" t="s">
         <v>195</v>
-      </c>
-      <c r="E164" s="40" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="165">
       <c r="A165" s="11"/>
       <c r="B165" s="11"/>
       <c r="C165" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D165" s="11"/>
       <c r="E165" s="11"/>
@@ -3940,7 +3937,7 @@
       <c r="A166" s="11"/>
       <c r="B166" s="11"/>
       <c r="C166" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D166" s="11"/>
       <c r="E166" s="11"/>
@@ -3949,7 +3946,7 @@
       <c r="A167" s="11"/>
       <c r="B167" s="11"/>
       <c r="C167" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D167" s="11"/>
       <c r="E167" s="11"/>
@@ -3958,7 +3955,7 @@
       <c r="A168" s="11"/>
       <c r="B168" s="11"/>
       <c r="C168" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D168" s="11"/>
       <c r="E168" s="11"/>
@@ -3967,7 +3964,7 @@
       <c r="A169" s="11"/>
       <c r="B169" s="11"/>
       <c r="C169" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D169" s="11"/>
       <c r="E169" s="11"/>
@@ -3976,7 +3973,7 @@
       <c r="A170" s="11"/>
       <c r="B170" s="11"/>
       <c r="C170" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D170" s="11"/>
       <c r="E170" s="11"/>
@@ -3985,7 +3982,7 @@
       <c r="A171" s="11"/>
       <c r="B171" s="11"/>
       <c r="C171" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D171" s="11"/>
       <c r="E171" s="11"/>
@@ -3994,7 +3991,7 @@
       <c r="A172" s="11"/>
       <c r="B172" s="11"/>
       <c r="C172" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D172" s="11"/>
       <c r="E172" s="11"/>
@@ -4003,7 +4000,7 @@
       <c r="A173" s="11"/>
       <c r="B173" s="11"/>
       <c r="C173" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D173" s="11"/>
       <c r="E173" s="11"/>
@@ -4012,7 +4009,7 @@
       <c r="A174" s="11"/>
       <c r="B174" s="11"/>
       <c r="C174" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D174" s="11"/>
       <c r="E174" s="11"/>
@@ -4021,7 +4018,7 @@
       <c r="A175" s="12"/>
       <c r="B175" s="12"/>
       <c r="C175" s="38" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D175" s="12"/>
       <c r="E175" s="12"/>
@@ -4031,7 +4028,7 @@
         <v>44.0</v>
       </c>
       <c r="B176" s="9" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C176" s="17" t="s">
         <v>27</v>
@@ -4040,7 +4037,7 @@
         <v>62</v>
       </c>
       <c r="E176" s="41" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="177">
@@ -4066,16 +4063,16 @@
         <v>45.0</v>
       </c>
       <c r="B179" s="20" t="s">
+        <v>198</v>
+      </c>
+      <c r="C179" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="C179" s="8" t="s">
+      <c r="D179" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="D179" s="8" t="s">
-        <v>201</v>
-      </c>
       <c r="E179" s="42" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="180">
@@ -4083,23 +4080,23 @@
         <v>46.0</v>
       </c>
       <c r="B180" s="17" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C180" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D180" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E180" s="40" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="181">
       <c r="A181" s="11"/>
       <c r="B181" s="11"/>
       <c r="C181" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D181" s="11"/>
       <c r="E181" s="11"/>
@@ -4108,7 +4105,7 @@
       <c r="A182" s="11"/>
       <c r="B182" s="11"/>
       <c r="C182" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D182" s="11"/>
       <c r="E182" s="11"/>
@@ -4117,7 +4114,7 @@
       <c r="A183" s="11"/>
       <c r="B183" s="11"/>
       <c r="C183" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D183" s="11"/>
       <c r="E183" s="11"/>
@@ -4126,7 +4123,7 @@
       <c r="A184" s="12"/>
       <c r="B184" s="12"/>
       <c r="C184" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D184" s="12"/>
       <c r="E184" s="12"/>
@@ -4136,16 +4133,16 @@
         <v>47.0</v>
       </c>
       <c r="B185" s="8" t="s">
+        <v>204</v>
+      </c>
+      <c r="C185" s="20" t="s">
         <v>205</v>
       </c>
-      <c r="C185" s="20" t="s">
+      <c r="D185" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="D185" s="8" t="s">
+      <c r="E185" s="42" t="s">
         <v>207</v>
-      </c>
-      <c r="E185" s="42" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="186">
@@ -4153,36 +4150,36 @@
         <v>48.0</v>
       </c>
       <c r="B186" s="17" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C186" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D186" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E186" s="10" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="187">
       <c r="B187" s="11"/>
       <c r="C187" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E187" s="11"/>
     </row>
     <row r="188">
       <c r="B188" s="11"/>
       <c r="C188" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E188" s="11"/>
     </row>
     <row r="189">
       <c r="B189" s="11"/>
       <c r="C189" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E189" s="11"/>
     </row>
@@ -4190,7 +4187,7 @@
       <c r="A190" s="35"/>
       <c r="B190" s="12"/>
       <c r="C190" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D190" s="35"/>
       <c r="E190" s="12"/>
@@ -4200,23 +4197,23 @@
         <v>49.0</v>
       </c>
       <c r="B191" s="17" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C191" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D191" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E191" s="27" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
     </row>
     <row r="192">
       <c r="A192" s="11"/>
       <c r="B192" s="11"/>
       <c r="C192" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D192" s="11"/>
       <c r="E192" s="11"/>
@@ -4225,7 +4222,7 @@
       <c r="A193" s="11"/>
       <c r="B193" s="11"/>
       <c r="C193" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D193" s="11"/>
       <c r="E193" s="11"/>
@@ -4234,7 +4231,7 @@
       <c r="A194" s="11"/>
       <c r="B194" s="11"/>
       <c r="C194" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D194" s="11"/>
       <c r="E194" s="11"/>
@@ -4243,7 +4240,7 @@
       <c r="A195" s="11"/>
       <c r="B195" s="11"/>
       <c r="C195" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D195" s="11"/>
       <c r="E195" s="11"/>
@@ -4252,7 +4249,7 @@
       <c r="A196" s="11"/>
       <c r="B196" s="11"/>
       <c r="C196" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D196" s="11"/>
       <c r="E196" s="11"/>
@@ -4261,7 +4258,7 @@
       <c r="A197" s="11"/>
       <c r="B197" s="11"/>
       <c r="C197" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D197" s="11"/>
       <c r="E197" s="11"/>
@@ -4270,7 +4267,7 @@
       <c r="A198" s="11"/>
       <c r="B198" s="11"/>
       <c r="C198" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D198" s="11"/>
       <c r="E198" s="11"/>
@@ -4279,7 +4276,7 @@
       <c r="A199" s="11"/>
       <c r="B199" s="11"/>
       <c r="C199" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D199" s="11"/>
       <c r="E199" s="11"/>
@@ -4288,7 +4285,7 @@
       <c r="A200" s="11"/>
       <c r="B200" s="11"/>
       <c r="C200" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D200" s="11"/>
       <c r="E200" s="11"/>
@@ -4297,7 +4294,7 @@
       <c r="A201" s="11"/>
       <c r="B201" s="11"/>
       <c r="C201" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D201" s="11"/>
       <c r="E201" s="11"/>
@@ -4306,7 +4303,7 @@
       <c r="A202" s="12"/>
       <c r="B202" s="12"/>
       <c r="C202" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D202" s="12"/>
       <c r="E202" s="12"/>
@@ -4316,22 +4313,22 @@
         <v>50.0</v>
       </c>
       <c r="B203" s="17" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="C203" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D203" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E203" s="40" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="204">
       <c r="B204" s="11"/>
       <c r="C204" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D204" s="11"/>
       <c r="E204" s="11"/>
@@ -4339,7 +4336,7 @@
     <row r="205">
       <c r="B205" s="11"/>
       <c r="C205" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D205" s="11"/>
       <c r="E205" s="11"/>
@@ -4347,7 +4344,7 @@
     <row r="206">
       <c r="B206" s="11"/>
       <c r="C206" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D206" s="11"/>
       <c r="E206" s="11"/>
@@ -4356,7 +4353,7 @@
       <c r="A207" s="35"/>
       <c r="B207" s="12"/>
       <c r="C207" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D207" s="12"/>
       <c r="E207" s="12"/>
@@ -4366,16 +4363,16 @@
         <v>51.0</v>
       </c>
       <c r="B208" s="8" t="s">
+        <v>216</v>
+      </c>
+      <c r="C208" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D208" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E208" s="42" t="s">
         <v>217</v>
-      </c>
-      <c r="C208" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D208" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E208" s="42" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="209">
@@ -4383,43 +4380,43 @@
         <v>52.0</v>
       </c>
       <c r="B209" s="17" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C209" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D209" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E209" s="10" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="210">
       <c r="B210" s="11"/>
       <c r="C210" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E210" s="11"/>
     </row>
     <row r="211">
       <c r="B211" s="11"/>
       <c r="C211" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E211" s="11"/>
     </row>
     <row r="212">
       <c r="B212" s="11"/>
       <c r="C212" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E212" s="11"/>
     </row>
     <row r="213">
       <c r="B213" s="12"/>
       <c r="C213" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D213" s="35"/>
       <c r="E213" s="12"/>
@@ -4429,22 +4426,22 @@
         <v>53.0</v>
       </c>
       <c r="B214" s="17" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="C214" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D214" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E214" s="27" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="215">
       <c r="B215" s="11"/>
       <c r="C215" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D215" s="11"/>
       <c r="E215" s="11"/>
@@ -4452,7 +4449,7 @@
     <row r="216">
       <c r="B216" s="11"/>
       <c r="C216" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D216" s="11"/>
       <c r="E216" s="11"/>
@@ -4460,7 +4457,7 @@
     <row r="217">
       <c r="B217" s="11"/>
       <c r="C217" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D217" s="11"/>
       <c r="E217" s="11"/>
@@ -4468,7 +4465,7 @@
     <row r="218">
       <c r="B218" s="11"/>
       <c r="C218" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D218" s="11"/>
       <c r="E218" s="11"/>
@@ -4476,7 +4473,7 @@
     <row r="219">
       <c r="B219" s="11"/>
       <c r="C219" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D219" s="11"/>
       <c r="E219" s="11"/>
@@ -4484,7 +4481,7 @@
     <row r="220">
       <c r="B220" s="11"/>
       <c r="C220" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D220" s="11"/>
       <c r="E220" s="11"/>
@@ -4492,7 +4489,7 @@
     <row r="221">
       <c r="B221" s="11"/>
       <c r="C221" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D221" s="11"/>
       <c r="E221" s="11"/>
@@ -4500,7 +4497,7 @@
     <row r="222">
       <c r="B222" s="11"/>
       <c r="C222" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D222" s="11"/>
       <c r="E222" s="11"/>
@@ -4508,7 +4505,7 @@
     <row r="223">
       <c r="B223" s="11"/>
       <c r="C223" s="32" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D223" s="11"/>
       <c r="E223" s="11"/>
@@ -4516,7 +4513,7 @@
     <row r="224">
       <c r="B224" s="11"/>
       <c r="C224" s="32" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D224" s="11"/>
       <c r="E224" s="11"/>
@@ -4524,7 +4521,7 @@
     <row r="225">
       <c r="B225" s="12"/>
       <c r="C225" s="38" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D225" s="12"/>
       <c r="E225" s="12"/>
@@ -4534,22 +4531,22 @@
         <v>54.0</v>
       </c>
       <c r="B226" s="17" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C226" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D226" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E226" s="40" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="227">
       <c r="B227" s="11"/>
       <c r="C227" s="17" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D227" s="11"/>
       <c r="E227" s="11"/>
@@ -4557,7 +4554,7 @@
     <row r="228">
       <c r="B228" s="11"/>
       <c r="C228" s="17" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D228" s="11"/>
       <c r="E228" s="11"/>
@@ -4565,7 +4562,7 @@
     <row r="229">
       <c r="B229" s="11"/>
       <c r="C229" s="17" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D229" s="11"/>
       <c r="E229" s="11"/>
@@ -4574,7 +4571,7 @@
       <c r="A230" s="35"/>
       <c r="B230" s="12"/>
       <c r="C230" s="20" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D230" s="12"/>
       <c r="E230" s="12"/>
@@ -4584,16 +4581,16 @@
         <v>55.0</v>
       </c>
       <c r="B231" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="C231" s="20" t="s">
+        <v>205</v>
+      </c>
+      <c r="D231" s="8" t="s">
+        <v>206</v>
+      </c>
+      <c r="E231" s="42" t="s">
         <v>225</v>
-      </c>
-      <c r="C231" s="20" t="s">
-        <v>206</v>
-      </c>
-      <c r="D231" s="8" t="s">
-        <v>207</v>
-      </c>
-      <c r="E231" s="42" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="232">
@@ -4601,36 +4598,36 @@
         <v>56.0</v>
       </c>
       <c r="B232" s="17" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C232" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D232" s="36" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E232" s="10" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
     </row>
     <row r="233">
       <c r="B233" s="11"/>
       <c r="C233" s="17" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="E233" s="11"/>
     </row>
     <row r="234">
       <c r="B234" s="11"/>
       <c r="C234" s="17" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E234" s="11"/>
     </row>
     <row r="235">
       <c r="B235" s="11"/>
       <c r="C235" s="17" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="E235" s="11"/>
     </row>
@@ -4638,7 +4635,7 @@
       <c r="A236" s="35"/>
       <c r="B236" s="12"/>
       <c r="C236" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D236" s="35"/>
       <c r="E236" s="12"/>
@@ -4648,23 +4645,23 @@
         <v>57.0</v>
       </c>
       <c r="B237" s="17" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C237" s="46" t="s">
         <v>27</v>
       </c>
       <c r="D237" s="9" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E237" s="27" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="238">
       <c r="A238" s="11"/>
       <c r="B238" s="11"/>
       <c r="C238" s="32" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D238" s="11"/>
       <c r="E238" s="11"/>
@@ -4673,7 +4670,7 @@
       <c r="A239" s="11"/>
       <c r="B239" s="11"/>
       <c r="C239" s="32" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D239" s="11"/>
       <c r="E239" s="11"/>
@@ -4682,7 +4679,7 @@
       <c r="A240" s="11"/>
       <c r="B240" s="11"/>
       <c r="C240" s="32" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D240" s="11"/>
       <c r="E240" s="11"/>
@@ -4691,7 +4688,7 @@
       <c r="A241" s="11"/>
       <c r="B241" s="11"/>
       <c r="C241" s="32" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D241" s="11"/>
       <c r="E241" s="11"/>
@@ -4700,7 +4697,7 @@
       <c r="A242" s="11"/>
       <c r="B242" s="11"/>
       <c r="C242" s="32" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D242" s="11"/>
       <c r="E242" s="11"/>
@@ -4709,7 +4706,7 @@
       <c r="A243" s="11"/>
       <c r="B243" s="11"/>
       <c r="C243" s="32" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D243" s="11"/>
       <c r="E243" s="11"/>
@@ -4718,7 +4715,7 @@
       <c r="A244" s="11"/>
       <c r="B244" s="11"/>
       <c r="C244" s="32" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D244" s="11"/>
       <c r="E244" s="11"/>
@@ -4727,7 +4724,7 @@
       <c r="A245" s="11"/>
       <c r="B245" s="11"/>
       <c r="C245" s="32" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D245" s="11"/>
       <c r="E245" s="11"/>
@@ -4736,7 +4733,7 @@
       <c r="A246" s="11"/>
       <c r="B246" s="11"/>
       <c r="C246" s="47" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D246" s="11"/>
       <c r="E246" s="11"/>
@@ -4745,7 +4742,7 @@
       <c r="A247" s="11"/>
       <c r="B247" s="11"/>
       <c r="C247" s="17" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D247" s="11"/>
       <c r="E247" s="11"/>
@@ -4754,7 +4751,7 @@
       <c r="A248" s="12"/>
       <c r="B248" s="12"/>
       <c r="C248" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D248" s="12"/>
       <c r="E248" s="12"/>
@@ -4764,22 +4761,22 @@
         <v>58.0</v>
       </c>
       <c r="B249" s="17" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C249" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D249" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="E249" s="48" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="250">
       <c r="B250" s="11"/>
       <c r="C250" s="32" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="D250" s="11"/>
       <c r="E250" s="18"/>
@@ -4787,7 +4784,7 @@
     <row r="251">
       <c r="B251" s="11"/>
       <c r="C251" s="32" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D251" s="11"/>
       <c r="E251" s="18"/>
@@ -4795,7 +4792,7 @@
     <row r="252">
       <c r="B252" s="11"/>
       <c r="C252" s="32" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D252" s="11"/>
       <c r="E252" s="18"/>
@@ -4803,7 +4800,7 @@
     <row r="253">
       <c r="B253" s="12"/>
       <c r="C253" s="32" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="D253" s="12"/>
       <c r="E253" s="21"/>
@@ -4813,16 +4810,16 @@
         <v>59.0</v>
       </c>
       <c r="B254" s="20" t="s">
+        <v>232</v>
+      </c>
+      <c r="C254" s="8" t="s">
+        <v>205</v>
+      </c>
+      <c r="D254" s="20" t="s">
         <v>233</v>
       </c>
-      <c r="C254" s="8" t="s">
-        <v>206</v>
-      </c>
-      <c r="D254" s="20" t="s">
+      <c r="E254" s="49" t="s">
         <v>234</v>
-      </c>
-      <c r="E254" s="49" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="255">
@@ -4830,22 +4827,22 @@
         <v>60.0</v>
       </c>
       <c r="B255" s="17" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C255" s="32" t="s">
         <v>27</v>
       </c>
       <c r="D255" s="17" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="E255" s="48" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="256">
       <c r="B256" s="11"/>
       <c r="C256" s="32" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D256" s="11"/>
       <c r="E256" s="18"/>
@@ -4853,7 +4850,7 @@
     <row r="257">
       <c r="B257" s="11"/>
       <c r="C257" s="32" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="D257" s="11"/>
       <c r="E257" s="18"/>
@@ -4861,7 +4858,7 @@
     <row r="258">
       <c r="B258" s="11"/>
       <c r="C258" s="32" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="D258" s="11"/>
       <c r="E258" s="18"/>
@@ -4869,7 +4866,7 @@
     <row r="259">
       <c r="B259" s="12"/>
       <c r="C259" s="32" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D259" s="12"/>
       <c r="E259" s="21"/>
@@ -4879,23 +4876,23 @@
         <v>61.0</v>
       </c>
       <c r="B260" s="17" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C260" s="50" t="s">
         <v>27</v>
       </c>
       <c r="D260" s="47" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="E260" s="48" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="261">
       <c r="A261" s="11"/>
       <c r="B261" s="11"/>
       <c r="C261" s="51" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="D261" s="11"/>
       <c r="E261" s="18"/>
@@ -4904,7 +4901,7 @@
       <c r="A262" s="11"/>
       <c r="B262" s="11"/>
       <c r="C262" s="51" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="D262" s="11"/>
       <c r="E262" s="18"/>
@@ -4913,7 +4910,7 @@
       <c r="A263" s="11"/>
       <c r="B263" s="11"/>
       <c r="C263" s="51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="D263" s="11"/>
       <c r="E263" s="18"/>
@@ -4922,7 +4919,7 @@
       <c r="A264" s="11"/>
       <c r="B264" s="11"/>
       <c r="C264" s="51" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="D264" s="11"/>
       <c r="E264" s="18"/>
@@ -4931,7 +4928,7 @@
       <c r="A265" s="11"/>
       <c r="B265" s="11"/>
       <c r="C265" s="51" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="D265" s="11"/>
       <c r="E265" s="18"/>
@@ -4940,7 +4937,7 @@
       <c r="A266" s="11"/>
       <c r="B266" s="11"/>
       <c r="C266" s="51" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D266" s="11"/>
       <c r="E266" s="18"/>
@@ -4949,7 +4946,7 @@
       <c r="A267" s="11"/>
       <c r="B267" s="11"/>
       <c r="C267" s="51" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="D267" s="11"/>
       <c r="E267" s="18"/>
@@ -4958,7 +4955,7 @@
       <c r="A268" s="11"/>
       <c r="B268" s="11"/>
       <c r="C268" s="51" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="D268" s="11"/>
       <c r="E268" s="18"/>
@@ -4967,7 +4964,7 @@
       <c r="A269" s="11"/>
       <c r="B269" s="11"/>
       <c r="C269" s="52" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="D269" s="11"/>
       <c r="E269" s="18"/>
@@ -4976,7 +4973,7 @@
       <c r="A270" s="11"/>
       <c r="B270" s="11"/>
       <c r="C270" s="52" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="D270" s="11"/>
       <c r="E270" s="18"/>
@@ -4985,14 +4982,14 @@
       <c r="A271" s="12"/>
       <c r="B271" s="12"/>
       <c r="C271" s="53" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D271" s="12"/>
       <c r="E271" s="21"/>
     </row>
     <row r="272" ht="24.75" customHeight="1">
       <c r="A272" s="54" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B272" s="4"/>
       <c r="C272" s="4"/>
@@ -5004,13 +5001,13 @@
         <v>62.0</v>
       </c>
       <c r="B273" s="9" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C273" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D273" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E273" s="10" t="s">
         <v>9</v>
@@ -5020,7 +5017,7 @@
       <c r="A274" s="11"/>
       <c r="B274" s="11"/>
       <c r="C274" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D274" s="11"/>
       <c r="E274" s="11"/>
@@ -5029,7 +5026,7 @@
       <c r="A275" s="11"/>
       <c r="B275" s="11"/>
       <c r="C275" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D275" s="11"/>
       <c r="E275" s="11"/>
@@ -5038,7 +5035,7 @@
       <c r="A276" s="11"/>
       <c r="B276" s="11"/>
       <c r="C276" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D276" s="11"/>
       <c r="E276" s="11"/>
@@ -5047,7 +5044,7 @@
       <c r="A277" s="11"/>
       <c r="B277" s="11"/>
       <c r="C277" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D277" s="11"/>
       <c r="E277" s="11"/>
@@ -5056,7 +5053,7 @@
       <c r="A278" s="11"/>
       <c r="B278" s="11"/>
       <c r="C278" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D278" s="11"/>
       <c r="E278" s="11"/>
@@ -5065,7 +5062,7 @@
       <c r="A279" s="11"/>
       <c r="B279" s="11"/>
       <c r="C279" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D279" s="11"/>
       <c r="E279" s="11"/>
@@ -5074,7 +5071,7 @@
       <c r="A280" s="11"/>
       <c r="B280" s="11"/>
       <c r="C280" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D280" s="11"/>
       <c r="E280" s="11"/>
@@ -5092,7 +5089,7 @@
       <c r="A282" s="12"/>
       <c r="B282" s="12"/>
       <c r="C282" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D282" s="12"/>
       <c r="E282" s="12"/>
@@ -5102,13 +5099,13 @@
         <v>63.0</v>
       </c>
       <c r="B283" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C283" s="17" t="s">
         <v>251</v>
       </c>
-      <c r="C283" s="17" t="s">
+      <c r="D283" s="17" t="s">
         <v>252</v>
-      </c>
-      <c r="D283" s="17" t="s">
-        <v>253</v>
       </c>
       <c r="E283" s="10" t="s">
         <v>9</v>
@@ -5146,23 +5143,23 @@
         <v>64.0</v>
       </c>
       <c r="B287" s="56" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C287" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D287" s="58" t="s">
         <v>102</v>
       </c>
       <c r="E287" s="59" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="288">
       <c r="A288" s="12"/>
       <c r="B288" s="35"/>
       <c r="C288" s="17" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="D288" s="18"/>
       <c r="E288" s="11"/>
@@ -5172,10 +5169,10 @@
         <v>65.0</v>
       </c>
       <c r="B289" s="60" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="C289" s="57" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D289" s="58" t="s">
         <v>106</v>
@@ -5186,7 +5183,7 @@
       <c r="A290" s="12"/>
       <c r="B290" s="19"/>
       <c r="C290" s="61" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="D290" s="18"/>
       <c r="E290" s="12"/>
@@ -5196,10 +5193,10 @@
         <v>66.0</v>
       </c>
       <c r="B291" s="14" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="C291" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D291" s="15" t="s">
         <v>109</v>
@@ -5212,7 +5209,7 @@
       <c r="A292" s="12"/>
       <c r="B292" s="19"/>
       <c r="C292" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="D292" s="21"/>
       <c r="E292" s="12"/>
@@ -5222,13 +5219,13 @@
         <v>67.0</v>
       </c>
       <c r="B293" s="17" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C293" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D293" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E293" s="27" t="s">
         <v>13</v>
@@ -5247,7 +5244,7 @@
       <c r="A295" s="12"/>
       <c r="B295" s="12"/>
       <c r="C295" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D295" s="12"/>
       <c r="E295" s="11"/>
@@ -5257,13 +5254,13 @@
         <v>68.0</v>
       </c>
       <c r="B296" s="17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="C296" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D296" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E296" s="11"/>
     </row>
@@ -5280,7 +5277,7 @@
       <c r="A298" s="12"/>
       <c r="B298" s="12"/>
       <c r="C298" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D298" s="12"/>
       <c r="E298" s="11"/>
@@ -5290,13 +5287,13 @@
         <v>69.0</v>
       </c>
       <c r="B299" s="17" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="C299" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D299" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E299" s="11"/>
     </row>
@@ -5313,7 +5310,7 @@
       <c r="A301" s="12"/>
       <c r="B301" s="12"/>
       <c r="C301" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D301" s="12"/>
       <c r="E301" s="11"/>
@@ -5323,13 +5320,13 @@
         <v>70.0</v>
       </c>
       <c r="B302" s="17" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="C302" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D302" s="17" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="E302" s="11"/>
     </row>
@@ -5346,7 +5343,7 @@
       <c r="A304" s="12"/>
       <c r="B304" s="12"/>
       <c r="C304" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="D304" s="12"/>
       <c r="E304" s="12"/>
@@ -5356,7 +5353,7 @@
         <v>71.0</v>
       </c>
       <c r="B305" s="17" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="C305" s="17" t="s">
         <v>27</v>
@@ -5365,7 +5362,7 @@
         <v>26</v>
       </c>
       <c r="E305" s="27" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="306">
@@ -5400,23 +5397,23 @@
         <v>72.0</v>
       </c>
       <c r="B309" s="9" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="C309" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D309" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="E309" s="10" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="310">
       <c r="A310" s="11"/>
       <c r="B310" s="11"/>
       <c r="C310" s="17" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="D310" s="11"/>
       <c r="E310" s="11"/>
@@ -5425,7 +5422,7 @@
       <c r="A311" s="11"/>
       <c r="B311" s="11"/>
       <c r="C311" s="17" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D311" s="11"/>
       <c r="E311" s="11"/>
@@ -5434,7 +5431,7 @@
       <c r="A312" s="11"/>
       <c r="B312" s="11"/>
       <c r="C312" s="17" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D312" s="11"/>
       <c r="E312" s="11"/>
@@ -5443,7 +5440,7 @@
       <c r="A313" s="11"/>
       <c r="B313" s="11"/>
       <c r="C313" s="17" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="D313" s="11"/>
       <c r="E313" s="11"/>
@@ -5452,7 +5449,7 @@
       <c r="A314" s="11"/>
       <c r="B314" s="11"/>
       <c r="C314" s="55" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D314" s="11"/>
       <c r="E314" s="11"/>
@@ -5461,7 +5458,7 @@
       <c r="A315" s="11"/>
       <c r="B315" s="11"/>
       <c r="C315" s="17" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="D315" s="11"/>
       <c r="E315" s="11"/>
@@ -5470,7 +5467,7 @@
       <c r="A316" s="11"/>
       <c r="B316" s="11"/>
       <c r="C316" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="D316" s="11"/>
       <c r="E316" s="11"/>
@@ -5488,14 +5485,14 @@
       <c r="A318" s="12"/>
       <c r="B318" s="11"/>
       <c r="C318" s="20" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D318" s="11"/>
       <c r="E318" s="12"/>
     </row>
     <row r="319" ht="24.75" customHeight="1">
       <c r="A319" s="62" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B319" s="4"/>
       <c r="C319" s="4"/>
@@ -5507,13 +5504,13 @@
         <v>73.0</v>
       </c>
       <c r="B320" s="9" t="s">
+        <v>271</v>
+      </c>
+      <c r="C320" s="36" t="s">
         <v>272</v>
       </c>
-      <c r="C320" s="36" t="s">
+      <c r="D320" s="9" t="s">
         <v>273</v>
-      </c>
-      <c r="D320" s="9" t="s">
-        <v>274</v>
       </c>
       <c r="E320" s="10" t="s">
         <v>9</v>
@@ -5541,7 +5538,7 @@
       <c r="A323" s="11"/>
       <c r="B323" s="11"/>
       <c r="C323" s="17" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="D323" s="11"/>
       <c r="E323" s="11"/>
@@ -5550,7 +5547,7 @@
       <c r="A324" s="11"/>
       <c r="B324" s="11"/>
       <c r="C324" s="17" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="D324" s="11"/>
       <c r="E324" s="11"/>
@@ -5559,7 +5556,7 @@
       <c r="A325" s="11"/>
       <c r="B325" s="11"/>
       <c r="C325" s="17" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D325" s="11"/>
       <c r="E325" s="11"/>
@@ -5569,23 +5566,23 @@
         <v>74.0</v>
       </c>
       <c r="B326" s="9" t="s">
+        <v>277</v>
+      </c>
+      <c r="C326" s="9" t="s">
         <v>278</v>
       </c>
-      <c r="C326" s="9" t="s">
+      <c r="D326" s="9" t="s">
         <v>279</v>
       </c>
-      <c r="D326" s="9" t="s">
+      <c r="E326" s="10" t="s">
         <v>280</v>
-      </c>
-      <c r="E326" s="10" t="s">
-        <v>281</v>
       </c>
     </row>
     <row r="327">
       <c r="A327" s="11"/>
       <c r="B327" s="11"/>
       <c r="C327" s="17" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="D327" s="11"/>
       <c r="E327" s="11"/>
@@ -5594,7 +5591,7 @@
       <c r="A328" s="11"/>
       <c r="B328" s="11"/>
       <c r="C328" s="17" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="D328" s="11"/>
       <c r="E328" s="11"/>
@@ -5604,13 +5601,13 @@
         <v>75.0</v>
       </c>
       <c r="B329" s="9" t="s">
+        <v>283</v>
+      </c>
+      <c r="C329" s="56" t="s">
+        <v>272</v>
+      </c>
+      <c r="D329" s="9" t="s">
         <v>284</v>
-      </c>
-      <c r="C329" s="56" t="s">
-        <v>273</v>
-      </c>
-      <c r="D329" s="9" t="s">
-        <v>285</v>
       </c>
       <c r="E329" s="10" t="s">
         <v>9</v>
@@ -5629,7 +5626,7 @@
       <c r="A331" s="11"/>
       <c r="B331" s="11"/>
       <c r="C331" s="17" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="D331" s="11"/>
       <c r="E331" s="11"/>
@@ -5638,7 +5635,7 @@
       <c r="A332" s="11"/>
       <c r="B332" s="11"/>
       <c r="C332" s="17" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="D332" s="11"/>
       <c r="E332" s="11"/>
@@ -5647,7 +5644,7 @@
       <c r="A333" s="11"/>
       <c r="B333" s="11"/>
       <c r="C333" s="17" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="D333" s="11"/>
       <c r="E333" s="11"/>
@@ -5656,7 +5653,7 @@
       <c r="A334" s="11"/>
       <c r="B334" s="11"/>
       <c r="C334" s="20" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="D334" s="11"/>
       <c r="E334" s="11"/>
@@ -5666,10 +5663,10 @@
         <v>76.0</v>
       </c>
       <c r="B335" s="9" t="s">
+        <v>289</v>
+      </c>
+      <c r="C335" s="17" t="s">
         <v>290</v>
-      </c>
-      <c r="C335" s="17" t="s">
-        <v>291</v>
       </c>
       <c r="D335" s="9" t="s">
         <v>26</v>
@@ -5719,10 +5716,10 @@
         <v>77.0</v>
       </c>
       <c r="B340" s="9" t="s">
+        <v>291</v>
+      </c>
+      <c r="C340" s="17" t="s">
         <v>292</v>
-      </c>
-      <c r="C340" s="17" t="s">
-        <v>293</v>
       </c>
       <c r="D340" s="11"/>
       <c r="E340" s="11"/>
@@ -5765,7 +5762,7 @@
     </row>
     <row r="345" ht="24.75" customHeight="1">
       <c r="A345" s="63" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="B345" s="4"/>
       <c r="C345" s="4"/>
@@ -5777,13 +5774,13 @@
         <v>78.0</v>
       </c>
       <c r="B346" s="14" t="s">
+        <v>294</v>
+      </c>
+      <c r="C346" s="9" t="s">
         <v>295</v>
       </c>
-      <c r="C346" s="9" t="s">
+      <c r="D346" s="15" t="s">
         <v>296</v>
-      </c>
-      <c r="D346" s="15" t="s">
-        <v>297</v>
       </c>
       <c r="E346" s="27" t="s">
         <v>9</v>
@@ -5793,7 +5790,7 @@
       <c r="A347" s="12"/>
       <c r="B347" s="19"/>
       <c r="C347" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D347" s="18"/>
       <c r="E347" s="12"/>
@@ -5803,7 +5800,7 @@
         <v>79.0</v>
       </c>
       <c r="B348" s="9" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C348" s="9" t="s">
         <v>27</v>
@@ -5812,7 +5809,7 @@
         <v>62</v>
       </c>
       <c r="E348" s="10" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="349">
@@ -5838,23 +5835,23 @@
         <v>80.0</v>
       </c>
       <c r="B351" s="14" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="C351" s="9" t="s">
+        <v>295</v>
+      </c>
+      <c r="D351" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="D351" s="15" t="s">
-        <v>297</v>
-      </c>
       <c r="E351" s="10" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="352">
       <c r="A352" s="12"/>
       <c r="B352" s="19"/>
       <c r="C352" s="17" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D352" s="18"/>
       <c r="E352" s="12"/>
@@ -5864,7 +5861,7 @@
         <v>81.0</v>
       </c>
       <c r="B353" s="9" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="C353" s="9" t="s">
         <v>27</v>
@@ -5873,7 +5870,7 @@
         <v>62</v>
       </c>
       <c r="E353" s="10" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="354">
@@ -5899,13 +5896,13 @@
         <v>82.0</v>
       </c>
       <c r="B356" s="9" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="C356" s="17" t="s">
         <v>27</v>
       </c>
       <c r="D356" s="9" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="E356" s="10" t="s">
         <v>9</v>
@@ -5915,7 +5912,7 @@
       <c r="A357" s="11"/>
       <c r="B357" s="11"/>
       <c r="C357" s="17" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="D357" s="11"/>
       <c r="E357" s="11"/>
@@ -5924,7 +5921,7 @@
       <c r="A358" s="11"/>
       <c r="B358" s="11"/>
       <c r="C358" s="17" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="D358" s="11"/>
       <c r="E358" s="11"/>
@@ -5933,7 +5930,7 @@
       <c r="A359" s="11"/>
       <c r="B359" s="11"/>
       <c r="C359" s="17" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="D359" s="11"/>
       <c r="E359" s="11"/>
@@ -5942,7 +5939,7 @@
       <c r="A360" s="12"/>
       <c r="B360" s="12"/>
       <c r="C360" s="20" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="D360" s="12"/>
       <c r="E360" s="12"/>
@@ -5952,13 +5949,13 @@
         <v>83.0</v>
       </c>
       <c r="B361" s="28" t="s">
+        <v>309</v>
+      </c>
+      <c r="C361" s="64" t="s">
         <v>310</v>
       </c>
-      <c r="C361" s="64" t="s">
+      <c r="D361" s="8" t="s">
         <v>311</v>
-      </c>
-      <c r="D361" s="8" t="s">
-        <v>312</v>
       </c>
       <c r="E361" s="6" t="s">
         <v>9</v>
@@ -5969,7 +5966,7 @@
         <v>84.0</v>
       </c>
       <c r="B362" s="9" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="C362" s="17" t="s">
         <v>27</v>
@@ -6013,16 +6010,16 @@
         <v>85.0</v>
       </c>
       <c r="B366" s="13" t="s">
+        <v>313</v>
+      </c>
+      <c r="C366" s="17" t="s">
         <v>314</v>
-      </c>
-      <c r="C366" s="17" t="s">
-        <v>315</v>
       </c>
       <c r="D366" s="65" t="s">
         <v>26</v>
       </c>
       <c r="E366" s="48" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
     </row>
     <row r="367">
@@ -6059,7 +6056,7 @@
     </row>
     <row r="371" ht="24.75" customHeight="1">
       <c r="A371" s="66" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B371" s="4"/>
       <c r="C371" s="4"/>
@@ -6071,13 +6068,13 @@
         <v>86.0</v>
       </c>
       <c r="B372" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C372" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C372" s="9" t="s">
+      <c r="D372" s="15" t="s">
         <v>319</v>
-      </c>
-      <c r="D372" s="15" t="s">
-        <v>320</v>
       </c>
       <c r="E372" s="10" t="s">
         <v>33</v>
@@ -6087,7 +6084,7 @@
       <c r="A373" s="12"/>
       <c r="B373" s="12"/>
       <c r="C373" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D373" s="21"/>
       <c r="E373" s="12"/>
@@ -6097,10 +6094,10 @@
         <v>87.0</v>
       </c>
       <c r="B374" s="9" t="s">
+        <v>321</v>
+      </c>
+      <c r="C374" s="17" t="s">
         <v>322</v>
-      </c>
-      <c r="C374" s="17" t="s">
-        <v>323</v>
       </c>
       <c r="D374" s="9" t="s">
         <v>69</v>
@@ -6150,16 +6147,16 @@
         <v>88.0</v>
       </c>
       <c r="B379" s="8" t="s">
+        <v>323</v>
+      </c>
+      <c r="C379" s="8" t="s">
         <v>324</v>
       </c>
-      <c r="C379" s="8" t="s">
+      <c r="D379" s="8" t="s">
         <v>325</v>
       </c>
-      <c r="D379" s="8" t="s">
+      <c r="E379" s="10" t="s">
         <v>326</v>
-      </c>
-      <c r="E379" s="10" t="s">
-        <v>327</v>
       </c>
     </row>
     <row r="380">
@@ -6167,13 +6164,13 @@
         <v>89.0</v>
       </c>
       <c r="B380" s="8" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C380" s="8" t="s">
+        <v>324</v>
+      </c>
+      <c r="D380" s="8" t="s">
         <v>325</v>
-      </c>
-      <c r="D380" s="8" t="s">
-        <v>326</v>
       </c>
       <c r="E380" s="11"/>
     </row>
@@ -6182,7 +6179,7 @@
         <v>90.0</v>
       </c>
       <c r="B381" s="9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C381" s="17" t="s">
         <v>27</v>
@@ -6221,16 +6218,16 @@
         <v>91.0</v>
       </c>
       <c r="B385" s="9" t="s">
+        <v>329</v>
+      </c>
+      <c r="C385" s="17" t="s">
         <v>330</v>
-      </c>
-      <c r="C385" s="17" t="s">
-        <v>331</v>
       </c>
       <c r="D385" s="9" t="s">
         <v>62</v>
       </c>
       <c r="E385" s="10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
     </row>
     <row r="386">
@@ -6265,16 +6262,16 @@
         <v>92.0</v>
       </c>
       <c r="B389" s="9" t="s">
+        <v>332</v>
+      </c>
+      <c r="C389" s="9" t="s">
         <v>333</v>
-      </c>
-      <c r="C389" s="9" t="s">
-        <v>334</v>
       </c>
       <c r="D389" s="9" t="s">
         <v>16</v>
       </c>
       <c r="E389" s="10" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
     </row>
     <row r="390">
@@ -6308,7 +6305,7 @@
         <v>19</v>
       </c>
       <c r="D392" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E392" s="11"/>
     </row>
@@ -6317,10 +6314,10 @@
         <v>95.0</v>
       </c>
       <c r="B393" s="9" t="s">
+        <v>336</v>
+      </c>
+      <c r="C393" s="9" t="s">
         <v>337</v>
-      </c>
-      <c r="C393" s="9" t="s">
-        <v>338</v>
       </c>
       <c r="D393" s="9" t="s">
         <v>16</v>
@@ -6358,7 +6355,7 @@
         <v>19</v>
       </c>
       <c r="D396" s="8" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E396" s="12"/>
     </row>
@@ -6367,10 +6364,10 @@
         <v>98.0</v>
       </c>
       <c r="B397" s="9" t="s">
+        <v>338</v>
+      </c>
+      <c r="C397" s="9" t="s">
         <v>339</v>
-      </c>
-      <c r="C397" s="9" t="s">
-        <v>340</v>
       </c>
       <c r="D397" s="17" t="s">
         <v>26</v>
@@ -6420,7 +6417,7 @@
         <v>99.0</v>
       </c>
       <c r="B402" s="36" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C402" s="17" t="s">
         <v>27</v>
@@ -6451,16 +6448,16 @@
         <v>100.0</v>
       </c>
       <c r="B405" s="8" t="s">
+        <v>341</v>
+      </c>
+      <c r="C405" s="8" t="s">
         <v>342</v>
       </c>
-      <c r="C405" s="8" t="s">
+      <c r="D405" s="8" t="s">
         <v>343</v>
       </c>
-      <c r="D405" s="8" t="s">
+      <c r="E405" s="10" t="s">
         <v>344</v>
-      </c>
-      <c r="E405" s="10" t="s">
-        <v>345</v>
       </c>
     </row>
     <row r="406">
@@ -6468,7 +6465,7 @@
         <v>101.0</v>
       </c>
       <c r="B406" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="C406" s="17" t="s">
         <v>27</v>
@@ -6528,13 +6525,13 @@
         <v>102.0</v>
       </c>
       <c r="B412" s="9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="C412" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D412" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E412" s="11"/>
     </row>
@@ -6542,7 +6539,7 @@
       <c r="A413" s="11"/>
       <c r="B413" s="11"/>
       <c r="C413" s="69" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="D413" s="11"/>
       <c r="E413" s="11"/>
@@ -6551,7 +6548,7 @@
       <c r="A414" s="11"/>
       <c r="B414" s="11"/>
       <c r="C414" s="69" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="D414" s="11"/>
       <c r="E414" s="11"/>
@@ -6560,7 +6557,7 @@
       <c r="A415" s="11"/>
       <c r="B415" s="11"/>
       <c r="C415" s="69" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="D415" s="11"/>
       <c r="E415" s="11"/>
@@ -6578,7 +6575,7 @@
       <c r="A417" s="12"/>
       <c r="B417" s="12"/>
       <c r="C417" s="69" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="D417" s="12"/>
       <c r="E417" s="12"/>
@@ -6588,13 +6585,13 @@
         <v>103.0</v>
       </c>
       <c r="B418" s="14" t="s">
+        <v>352</v>
+      </c>
+      <c r="C418" s="9" t="s">
         <v>353</v>
       </c>
-      <c r="C418" s="9" t="s">
+      <c r="D418" s="15" t="s">
         <v>354</v>
-      </c>
-      <c r="D418" s="15" t="s">
-        <v>355</v>
       </c>
       <c r="E418" s="10" t="s">
         <v>33</v>
@@ -6604,7 +6601,7 @@
       <c r="A419" s="11"/>
       <c r="B419" s="16"/>
       <c r="C419" s="17" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D419" s="18"/>
       <c r="E419" s="11"/>
@@ -6614,13 +6611,13 @@
         <v>104.0</v>
       </c>
       <c r="B420" s="9" t="s">
+        <v>356</v>
+      </c>
+      <c r="C420" s="9" t="s">
         <v>357</v>
       </c>
-      <c r="C420" s="9" t="s">
-        <v>358</v>
-      </c>
       <c r="D420" s="9" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="E420" s="11"/>
     </row>
@@ -6628,7 +6625,7 @@
       <c r="A421" s="11"/>
       <c r="B421" s="11"/>
       <c r="C421" s="20" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="D421" s="11"/>
       <c r="E421" s="11"/>
@@ -6638,7 +6635,7 @@
         <v>105.0</v>
       </c>
       <c r="B422" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C422" s="17" t="s">
         <v>27</v>
@@ -6671,16 +6668,16 @@
         <v>106.0</v>
       </c>
       <c r="B425" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C425" s="9" t="s">
         <v>361</v>
       </c>
-      <c r="C425" s="9" t="s">
+      <c r="D425" s="9" t="s">
+        <v>354</v>
+      </c>
+      <c r="E425" s="6" t="s">
         <v>362</v>
-      </c>
-      <c r="D425" s="9" t="s">
-        <v>355</v>
-      </c>
-      <c r="E425" s="6" t="s">
-        <v>363</v>
       </c>
     </row>
     <row r="426">
@@ -6688,23 +6685,23 @@
         <v>107.0</v>
       </c>
       <c r="B426" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C426" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D426" s="9" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E426" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="427">
       <c r="A427" s="11"/>
       <c r="B427" s="11"/>
       <c r="C427" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D427" s="11"/>
       <c r="E427" s="11"/>
@@ -6713,7 +6710,7 @@
       <c r="A428" s="11"/>
       <c r="B428" s="11"/>
       <c r="C428" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D428" s="11"/>
       <c r="E428" s="11"/>
@@ -6722,7 +6719,7 @@
       <c r="A429" s="11"/>
       <c r="B429" s="11"/>
       <c r="C429" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D429" s="11"/>
       <c r="E429" s="11"/>
@@ -6731,7 +6728,7 @@
       <c r="A430" s="11"/>
       <c r="B430" s="11"/>
       <c r="C430" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D430" s="11"/>
       <c r="E430" s="11"/>
@@ -6740,7 +6737,7 @@
       <c r="A431" s="11"/>
       <c r="B431" s="11"/>
       <c r="C431" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D431" s="11"/>
       <c r="E431" s="11"/>
@@ -6749,7 +6746,7 @@
       <c r="A432" s="11"/>
       <c r="B432" s="11"/>
       <c r="C432" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D432" s="11"/>
       <c r="E432" s="11"/>
@@ -6758,7 +6755,7 @@
       <c r="A433" s="11"/>
       <c r="B433" s="11"/>
       <c r="C433" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D433" s="11"/>
       <c r="E433" s="11"/>
@@ -6767,7 +6764,7 @@
       <c r="A434" s="11"/>
       <c r="B434" s="11"/>
       <c r="C434" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D434" s="11"/>
       <c r="E434" s="11"/>
@@ -6776,7 +6773,7 @@
       <c r="A435" s="11"/>
       <c r="B435" s="11"/>
       <c r="C435" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D435" s="11"/>
       <c r="E435" s="11"/>
@@ -6785,7 +6782,7 @@
       <c r="A436" s="11"/>
       <c r="B436" s="11"/>
       <c r="C436" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D436" s="11"/>
       <c r="E436" s="11"/>
@@ -6794,7 +6791,7 @@
       <c r="A437" s="11"/>
       <c r="B437" s="11"/>
       <c r="C437" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D437" s="11"/>
       <c r="E437" s="11"/>
@@ -6803,7 +6800,7 @@
       <c r="A438" s="11"/>
       <c r="B438" s="11"/>
       <c r="C438" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D438" s="11"/>
       <c r="E438" s="11"/>
@@ -6812,7 +6809,7 @@
       <c r="A439" s="11"/>
       <c r="B439" s="11"/>
       <c r="C439" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D439" s="11"/>
       <c r="E439" s="11"/>
@@ -6821,7 +6818,7 @@
       <c r="A440" s="11"/>
       <c r="B440" s="11"/>
       <c r="C440" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D440" s="11"/>
       <c r="E440" s="11"/>
@@ -6830,7 +6827,7 @@
       <c r="A441" s="11"/>
       <c r="B441" s="11"/>
       <c r="C441" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D441" s="11"/>
       <c r="E441" s="11"/>
@@ -6839,7 +6836,7 @@
       <c r="A442" s="11"/>
       <c r="B442" s="11"/>
       <c r="C442" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D442" s="11"/>
       <c r="E442" s="11"/>
@@ -6848,7 +6845,7 @@
       <c r="A443" s="11"/>
       <c r="B443" s="11"/>
       <c r="C443" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D443" s="11"/>
       <c r="E443" s="11"/>
@@ -6857,7 +6854,7 @@
       <c r="A444" s="11"/>
       <c r="B444" s="11"/>
       <c r="C444" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D444" s="11"/>
       <c r="E444" s="11"/>
@@ -6866,7 +6863,7 @@
       <c r="A445" s="11"/>
       <c r="B445" s="11"/>
       <c r="C445" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D445" s="11"/>
       <c r="E445" s="11"/>
@@ -6875,7 +6872,7 @@
       <c r="A446" s="11"/>
       <c r="B446" s="11"/>
       <c r="C446" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D446" s="11"/>
       <c r="E446" s="11"/>
@@ -6884,7 +6881,7 @@
       <c r="A447" s="11"/>
       <c r="B447" s="11"/>
       <c r="C447" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D447" s="11"/>
       <c r="E447" s="11"/>
@@ -6893,7 +6890,7 @@
       <c r="A448" s="11"/>
       <c r="B448" s="11"/>
       <c r="C448" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D448" s="11"/>
       <c r="E448" s="11"/>
@@ -6902,7 +6899,7 @@
       <c r="A449" s="11"/>
       <c r="B449" s="11"/>
       <c r="C449" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D449" s="11"/>
       <c r="E449" s="11"/>
@@ -6911,7 +6908,7 @@
       <c r="A450" s="11"/>
       <c r="B450" s="11"/>
       <c r="C450" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D450" s="11"/>
       <c r="E450" s="11"/>
@@ -6920,7 +6917,7 @@
       <c r="A451" s="11"/>
       <c r="B451" s="11"/>
       <c r="C451" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D451" s="11"/>
       <c r="E451" s="11"/>
@@ -6929,7 +6926,7 @@
       <c r="A452" s="11"/>
       <c r="B452" s="11"/>
       <c r="C452" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D452" s="11"/>
       <c r="E452" s="11"/>
@@ -6938,7 +6935,7 @@
       <c r="A453" s="11"/>
       <c r="B453" s="11"/>
       <c r="C453" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D453" s="11"/>
       <c r="E453" s="11"/>
@@ -6947,7 +6944,7 @@
       <c r="A454" s="11"/>
       <c r="B454" s="11"/>
       <c r="C454" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D454" s="11"/>
       <c r="E454" s="11"/>
@@ -6956,7 +6953,7 @@
       <c r="A455" s="11"/>
       <c r="B455" s="11"/>
       <c r="C455" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D455" s="11"/>
       <c r="E455" s="11"/>
@@ -6965,7 +6962,7 @@
       <c r="A456" s="11"/>
       <c r="B456" s="11"/>
       <c r="C456" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D456" s="11"/>
       <c r="E456" s="11"/>
@@ -6974,7 +6971,7 @@
       <c r="A457" s="11"/>
       <c r="B457" s="11"/>
       <c r="C457" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D457" s="11"/>
       <c r="E457" s="11"/>
@@ -6983,7 +6980,7 @@
       <c r="A458" s="11"/>
       <c r="B458" s="11"/>
       <c r="C458" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D458" s="11"/>
       <c r="E458" s="11"/>
@@ -6992,7 +6989,7 @@
       <c r="A459" s="11"/>
       <c r="B459" s="11"/>
       <c r="C459" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D459" s="11"/>
       <c r="E459" s="11"/>
@@ -7001,7 +6998,7 @@
       <c r="A460" s="11"/>
       <c r="B460" s="11"/>
       <c r="C460" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D460" s="11"/>
       <c r="E460" s="11"/>
@@ -7010,7 +7007,7 @@
       <c r="A461" s="11"/>
       <c r="B461" s="11"/>
       <c r="C461" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D461" s="11"/>
       <c r="E461" s="11"/>
@@ -7019,7 +7016,7 @@
       <c r="A462" s="11"/>
       <c r="B462" s="11"/>
       <c r="C462" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D462" s="11"/>
       <c r="E462" s="11"/>
@@ -7028,7 +7025,7 @@
       <c r="A463" s="11"/>
       <c r="B463" s="11"/>
       <c r="C463" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D463" s="11"/>
       <c r="E463" s="11"/>
@@ -7037,7 +7034,7 @@
       <c r="A464" s="11"/>
       <c r="B464" s="11"/>
       <c r="C464" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D464" s="11"/>
       <c r="E464" s="11"/>
@@ -7046,7 +7043,7 @@
       <c r="A465" s="11"/>
       <c r="B465" s="11"/>
       <c r="C465" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D465" s="11"/>
       <c r="E465" s="11"/>
@@ -7055,7 +7052,7 @@
       <c r="A466" s="11"/>
       <c r="B466" s="11"/>
       <c r="C466" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D466" s="11"/>
       <c r="E466" s="11"/>
@@ -7065,16 +7062,16 @@
         <v>108.0</v>
       </c>
       <c r="B467" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C467" s="20" t="s">
         <v>406</v>
-      </c>
-      <c r="C467" s="20" t="s">
-        <v>407</v>
       </c>
       <c r="D467" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E467" s="10" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="468">
@@ -7082,16 +7079,16 @@
         <v>109.0</v>
       </c>
       <c r="B468" s="8" t="s">
+        <v>408</v>
+      </c>
+      <c r="C468" s="8" t="s">
         <v>409</v>
       </c>
-      <c r="C468" s="8" t="s">
+      <c r="D468" s="9" t="s">
         <v>410</v>
       </c>
-      <c r="D468" s="9" t="s">
-        <v>411</v>
-      </c>
       <c r="E468" s="10" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
     </row>
     <row r="469">
@@ -7099,10 +7096,10 @@
         <v>110.0</v>
       </c>
       <c r="B469" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C469" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C469" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D469" s="9" t="s">
         <v>26</v>
@@ -7140,7 +7137,7 @@
       <c r="A473" s="11"/>
       <c r="B473" s="11"/>
       <c r="C473" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D473" s="11"/>
       <c r="E473" s="11"/>
@@ -7150,13 +7147,13 @@
         <v>111.0</v>
       </c>
       <c r="B474" s="9" t="s">
+        <v>414</v>
+      </c>
+      <c r="C474" s="13" t="s">
         <v>415</v>
       </c>
-      <c r="C474" s="13" t="s">
-        <v>416</v>
-      </c>
       <c r="D474" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E474" s="10" t="s">
         <v>33</v>
@@ -7166,7 +7163,7 @@
       <c r="A475" s="12"/>
       <c r="B475" s="12"/>
       <c r="C475" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D475" s="11"/>
       <c r="E475" s="12"/>
@@ -7176,21 +7173,21 @@
         <v>112.0</v>
       </c>
       <c r="B476" s="14" t="s">
+        <v>417</v>
+      </c>
+      <c r="C476" s="9" t="s">
         <v>418</v>
-      </c>
-      <c r="C476" s="9" t="s">
-        <v>419</v>
       </c>
       <c r="D476" s="11"/>
       <c r="E476" s="10" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
     </row>
     <row r="477" ht="35.25" customHeight="1">
       <c r="A477" s="12"/>
       <c r="B477" s="19"/>
       <c r="C477" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D477" s="11"/>
       <c r="E477" s="12"/>
@@ -7200,13 +7197,13 @@
         <v>113.0</v>
       </c>
       <c r="B478" s="14" t="s">
+        <v>420</v>
+      </c>
+      <c r="C478" s="9" t="s">
         <v>421</v>
       </c>
-      <c r="C478" s="9" t="s">
+      <c r="D478" s="15" t="s">
         <v>422</v>
-      </c>
-      <c r="D478" s="15" t="s">
-        <v>423</v>
       </c>
       <c r="E478" s="10" t="s">
         <v>33</v>
@@ -7216,7 +7213,7 @@
       <c r="A479" s="12"/>
       <c r="B479" s="19"/>
       <c r="C479" s="17" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D479" s="21"/>
       <c r="E479" s="11"/>
@@ -7226,13 +7223,13 @@
         <v>114.0</v>
       </c>
       <c r="B480" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C480" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C480" s="9" t="s">
-        <v>426</v>
-      </c>
       <c r="D480" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E480" s="11"/>
     </row>
@@ -7240,14 +7237,14 @@
       <c r="A481" s="12"/>
       <c r="B481" s="19"/>
       <c r="C481" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D481" s="21"/>
       <c r="E481" s="12"/>
     </row>
     <row r="482" ht="23.25" customHeight="1">
       <c r="A482" s="70" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B482" s="4"/>
       <c r="C482" s="4"/>
@@ -7259,13 +7256,13 @@
         <v>115.0</v>
       </c>
       <c r="B483" s="9" t="s">
+        <v>317</v>
+      </c>
+      <c r="C483" s="9" t="s">
         <v>318</v>
       </c>
-      <c r="C483" s="9" t="s">
+      <c r="D483" s="9" t="s">
         <v>319</v>
-      </c>
-      <c r="D483" s="9" t="s">
-        <v>320</v>
       </c>
       <c r="E483" s="10" t="s">
         <v>44</v>
@@ -7275,7 +7272,7 @@
       <c r="A484" s="12"/>
       <c r="B484" s="12"/>
       <c r="C484" s="67" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="D484" s="12"/>
       <c r="E484" s="11"/>
@@ -7285,13 +7282,13 @@
         <v>116.0</v>
       </c>
       <c r="B485" s="14" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C485" s="17" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="D485" s="15" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E485" s="11"/>
     </row>
@@ -7299,7 +7296,7 @@
       <c r="A486" s="11"/>
       <c r="B486" s="16"/>
       <c r="C486" s="17" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D486" s="18"/>
       <c r="E486" s="12"/>
@@ -7309,16 +7306,16 @@
         <v>117.0</v>
       </c>
       <c r="B487" s="8" t="s">
+        <v>428</v>
+      </c>
+      <c r="C487" s="9" t="s">
         <v>429</v>
       </c>
-      <c r="C487" s="9" t="s">
+      <c r="D487" s="8" t="s">
+        <v>354</v>
+      </c>
+      <c r="E487" s="6" t="s">
         <v>430</v>
-      </c>
-      <c r="D487" s="8" t="s">
-        <v>355</v>
-      </c>
-      <c r="E487" s="6" t="s">
-        <v>431</v>
       </c>
     </row>
     <row r="488">
@@ -7326,16 +7323,16 @@
         <v>118.0</v>
       </c>
       <c r="B488" s="71" t="s">
+        <v>431</v>
+      </c>
+      <c r="C488" s="9" t="s">
         <v>432</v>
       </c>
-      <c r="C488" s="9" t="s">
+      <c r="D488" s="28" t="s">
+        <v>325</v>
+      </c>
+      <c r="E488" s="6" t="s">
         <v>433</v>
-      </c>
-      <c r="D488" s="28" t="s">
-        <v>326</v>
-      </c>
-      <c r="E488" s="6" t="s">
-        <v>434</v>
       </c>
     </row>
     <row r="489">
@@ -7343,7 +7340,7 @@
         <v>119.0</v>
       </c>
       <c r="B489" s="65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C489" s="9" t="s">
         <v>27</v>
@@ -7352,7 +7349,7 @@
         <v>62</v>
       </c>
       <c r="E489" s="10" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
     </row>
     <row r="490">
@@ -7378,16 +7375,16 @@
         <v>120.0</v>
       </c>
       <c r="B492" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C492" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C492" s="13" t="s">
-        <v>362</v>
-      </c>
       <c r="D492" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E492" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="493">
@@ -7395,23 +7392,23 @@
         <v>121.0</v>
       </c>
       <c r="B493" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C493" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D493" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E493" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="494">
       <c r="A494" s="11"/>
       <c r="B494" s="11"/>
       <c r="C494" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D494" s="11"/>
       <c r="E494" s="11"/>
@@ -7420,7 +7417,7 @@
       <c r="A495" s="11"/>
       <c r="B495" s="11"/>
       <c r="C495" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D495" s="11"/>
       <c r="E495" s="11"/>
@@ -7429,7 +7426,7 @@
       <c r="A496" s="11"/>
       <c r="B496" s="11"/>
       <c r="C496" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D496" s="11"/>
       <c r="E496" s="11"/>
@@ -7438,7 +7435,7 @@
       <c r="A497" s="11"/>
       <c r="B497" s="11"/>
       <c r="C497" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D497" s="11"/>
       <c r="E497" s="11"/>
@@ -7447,7 +7444,7 @@
       <c r="A498" s="11"/>
       <c r="B498" s="11"/>
       <c r="C498" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D498" s="11"/>
       <c r="E498" s="11"/>
@@ -7456,7 +7453,7 @@
       <c r="A499" s="11"/>
       <c r="B499" s="11"/>
       <c r="C499" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D499" s="11"/>
       <c r="E499" s="11"/>
@@ -7465,7 +7462,7 @@
       <c r="A500" s="11"/>
       <c r="B500" s="11"/>
       <c r="C500" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D500" s="11"/>
       <c r="E500" s="11"/>
@@ -7474,7 +7471,7 @@
       <c r="A501" s="11"/>
       <c r="B501" s="11"/>
       <c r="C501" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D501" s="11"/>
       <c r="E501" s="11"/>
@@ -7483,7 +7480,7 @@
       <c r="A502" s="11"/>
       <c r="B502" s="11"/>
       <c r="C502" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D502" s="11"/>
       <c r="E502" s="11"/>
@@ -7492,7 +7489,7 @@
       <c r="A503" s="11"/>
       <c r="B503" s="11"/>
       <c r="C503" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D503" s="11"/>
       <c r="E503" s="11"/>
@@ -7501,7 +7498,7 @@
       <c r="A504" s="11"/>
       <c r="B504" s="11"/>
       <c r="C504" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D504" s="11"/>
       <c r="E504" s="11"/>
@@ -7510,7 +7507,7 @@
       <c r="A505" s="11"/>
       <c r="B505" s="11"/>
       <c r="C505" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D505" s="11"/>
       <c r="E505" s="11"/>
@@ -7519,7 +7516,7 @@
       <c r="A506" s="11"/>
       <c r="B506" s="11"/>
       <c r="C506" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D506" s="11"/>
       <c r="E506" s="11"/>
@@ -7528,7 +7525,7 @@
       <c r="A507" s="11"/>
       <c r="B507" s="11"/>
       <c r="C507" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D507" s="11"/>
       <c r="E507" s="11"/>
@@ -7537,7 +7534,7 @@
       <c r="A508" s="11"/>
       <c r="B508" s="11"/>
       <c r="C508" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D508" s="11"/>
       <c r="E508" s="11"/>
@@ -7546,7 +7543,7 @@
       <c r="A509" s="11"/>
       <c r="B509" s="11"/>
       <c r="C509" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D509" s="11"/>
       <c r="E509" s="11"/>
@@ -7555,7 +7552,7 @@
       <c r="A510" s="11"/>
       <c r="B510" s="11"/>
       <c r="C510" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D510" s="11"/>
       <c r="E510" s="11"/>
@@ -7564,7 +7561,7 @@
       <c r="A511" s="11"/>
       <c r="B511" s="11"/>
       <c r="C511" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D511" s="11"/>
       <c r="E511" s="11"/>
@@ -7573,7 +7570,7 @@
       <c r="A512" s="11"/>
       <c r="B512" s="11"/>
       <c r="C512" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D512" s="11"/>
       <c r="E512" s="11"/>
@@ -7582,7 +7579,7 @@
       <c r="A513" s="11"/>
       <c r="B513" s="11"/>
       <c r="C513" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D513" s="11"/>
       <c r="E513" s="11"/>
@@ -7591,7 +7588,7 @@
       <c r="A514" s="11"/>
       <c r="B514" s="11"/>
       <c r="C514" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D514" s="11"/>
       <c r="E514" s="11"/>
@@ -7600,7 +7597,7 @@
       <c r="A515" s="11"/>
       <c r="B515" s="11"/>
       <c r="C515" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D515" s="11"/>
       <c r="E515" s="11"/>
@@ -7609,7 +7606,7 @@
       <c r="A516" s="11"/>
       <c r="B516" s="11"/>
       <c r="C516" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D516" s="11"/>
       <c r="E516" s="11"/>
@@ -7618,7 +7615,7 @@
       <c r="A517" s="11"/>
       <c r="B517" s="11"/>
       <c r="C517" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D517" s="11"/>
       <c r="E517" s="11"/>
@@ -7627,7 +7624,7 @@
       <c r="A518" s="11"/>
       <c r="B518" s="11"/>
       <c r="C518" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D518" s="11"/>
       <c r="E518" s="11"/>
@@ -7636,7 +7633,7 @@
       <c r="A519" s="11"/>
       <c r="B519" s="11"/>
       <c r="C519" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D519" s="11"/>
       <c r="E519" s="11"/>
@@ -7645,7 +7642,7 @@
       <c r="A520" s="11"/>
       <c r="B520" s="11"/>
       <c r="C520" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D520" s="11"/>
       <c r="E520" s="11"/>
@@ -7654,7 +7651,7 @@
       <c r="A521" s="11"/>
       <c r="B521" s="11"/>
       <c r="C521" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D521" s="11"/>
       <c r="E521" s="11"/>
@@ -7663,7 +7660,7 @@
       <c r="A522" s="11"/>
       <c r="B522" s="11"/>
       <c r="C522" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D522" s="11"/>
       <c r="E522" s="11"/>
@@ -7672,7 +7669,7 @@
       <c r="A523" s="11"/>
       <c r="B523" s="11"/>
       <c r="C523" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D523" s="11"/>
       <c r="E523" s="11"/>
@@ -7681,7 +7678,7 @@
       <c r="A524" s="11"/>
       <c r="B524" s="11"/>
       <c r="C524" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D524" s="11"/>
       <c r="E524" s="11"/>
@@ -7690,7 +7687,7 @@
       <c r="A525" s="11"/>
       <c r="B525" s="11"/>
       <c r="C525" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D525" s="11"/>
       <c r="E525" s="11"/>
@@ -7699,7 +7696,7 @@
       <c r="A526" s="11"/>
       <c r="B526" s="11"/>
       <c r="C526" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D526" s="11"/>
       <c r="E526" s="11"/>
@@ -7708,7 +7705,7 @@
       <c r="A527" s="11"/>
       <c r="B527" s="11"/>
       <c r="C527" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D527" s="11"/>
       <c r="E527" s="11"/>
@@ -7717,7 +7714,7 @@
       <c r="A528" s="11"/>
       <c r="B528" s="11"/>
       <c r="C528" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D528" s="11"/>
       <c r="E528" s="11"/>
@@ -7726,7 +7723,7 @@
       <c r="A529" s="11"/>
       <c r="B529" s="11"/>
       <c r="C529" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D529" s="11"/>
       <c r="E529" s="11"/>
@@ -7735,7 +7732,7 @@
       <c r="A530" s="11"/>
       <c r="B530" s="11"/>
       <c r="C530" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D530" s="11"/>
       <c r="E530" s="11"/>
@@ -7744,7 +7741,7 @@
       <c r="A531" s="11"/>
       <c r="B531" s="11"/>
       <c r="C531" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D531" s="11"/>
       <c r="E531" s="11"/>
@@ -7753,7 +7750,7 @@
       <c r="A532" s="11"/>
       <c r="B532" s="11"/>
       <c r="C532" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D532" s="11"/>
       <c r="E532" s="11"/>
@@ -7762,7 +7759,7 @@
       <c r="A533" s="11"/>
       <c r="B533" s="11"/>
       <c r="C533" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D533" s="11"/>
       <c r="E533" s="11"/>
@@ -7772,16 +7769,16 @@
         <v>122.0</v>
       </c>
       <c r="B534" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C534" s="64" t="s">
         <v>406</v>
-      </c>
-      <c r="C534" s="64" t="s">
-        <v>407</v>
       </c>
       <c r="D534" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E534" s="6" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
     </row>
     <row r="535">
@@ -7789,16 +7786,16 @@
         <v>123.0</v>
       </c>
       <c r="B535" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C535" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D535" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E535" s="10" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
     </row>
     <row r="536">
@@ -7806,10 +7803,10 @@
         <v>124.0</v>
       </c>
       <c r="B536" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C536" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C536" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D536" s="9" t="s">
         <v>26</v>
@@ -7847,7 +7844,7 @@
       <c r="A540" s="11"/>
       <c r="B540" s="11"/>
       <c r="C540" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D540" s="11"/>
       <c r="E540" s="11"/>
@@ -7857,13 +7854,13 @@
         <v>125.0</v>
       </c>
       <c r="B541" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C541" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D541" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E541" s="10" t="s">
         <v>44</v>
@@ -7873,7 +7870,7 @@
       <c r="A542" s="11"/>
       <c r="B542" s="11"/>
       <c r="C542" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D542" s="11"/>
       <c r="E542" s="11"/>
@@ -7883,13 +7880,13 @@
         <v>126.0</v>
       </c>
       <c r="B543" s="9" t="s">
+        <v>424</v>
+      </c>
+      <c r="C543" s="9" t="s">
         <v>425</v>
       </c>
-      <c r="C543" s="9" t="s">
-        <v>426</v>
-      </c>
       <c r="D543" s="24" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E543" s="11"/>
     </row>
@@ -7897,14 +7894,14 @@
       <c r="A544" s="12"/>
       <c r="B544" s="12"/>
       <c r="C544" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D544" s="12"/>
       <c r="E544" s="12"/>
     </row>
     <row r="545" ht="22.5" customHeight="1">
       <c r="A545" s="70" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B545" s="4"/>
       <c r="C545" s="4"/>
@@ -7916,13 +7913,13 @@
         <v>127.0</v>
       </c>
       <c r="B546" s="8" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="C546" s="8" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="D546" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E546" s="10" t="s">
         <v>54</v>
@@ -7933,7 +7930,7 @@
         <v>128.0</v>
       </c>
       <c r="B547" s="65" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="C547" s="17" t="s">
         <v>27</v>
@@ -7966,16 +7963,16 @@
         <v>129.0</v>
       </c>
       <c r="B550" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="C550" s="13" t="s">
         <v>361</v>
       </c>
-      <c r="C550" s="13" t="s">
-        <v>362</v>
-      </c>
       <c r="D550" s="8" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E550" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="551">
@@ -7983,23 +7980,23 @@
         <v>130.0</v>
       </c>
       <c r="B551" s="9" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="C551" s="9" t="s">
         <v>27</v>
       </c>
       <c r="D551" s="9" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="E551" s="10" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="552">
       <c r="A552" s="11"/>
       <c r="B552" s="11"/>
       <c r="C552" s="17" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="D552" s="11"/>
       <c r="E552" s="11"/>
@@ -8008,7 +8005,7 @@
       <c r="A553" s="11"/>
       <c r="B553" s="11"/>
       <c r="C553" s="17" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="D553" s="11"/>
       <c r="E553" s="11"/>
@@ -8017,7 +8014,7 @@
       <c r="A554" s="11"/>
       <c r="B554" s="11"/>
       <c r="C554" s="17" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="D554" s="11"/>
       <c r="E554" s="11"/>
@@ -8026,7 +8023,7 @@
       <c r="A555" s="11"/>
       <c r="B555" s="11"/>
       <c r="C555" s="17" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="D555" s="11"/>
       <c r="E555" s="11"/>
@@ -8035,7 +8032,7 @@
       <c r="A556" s="11"/>
       <c r="B556" s="11"/>
       <c r="C556" s="17" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="D556" s="11"/>
       <c r="E556" s="11"/>
@@ -8044,7 +8041,7 @@
       <c r="A557" s="11"/>
       <c r="B557" s="11"/>
       <c r="C557" s="17" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="D557" s="11"/>
       <c r="E557" s="11"/>
@@ -8053,7 +8050,7 @@
       <c r="A558" s="11"/>
       <c r="B558" s="11"/>
       <c r="C558" s="17" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="D558" s="11"/>
       <c r="E558" s="11"/>
@@ -8062,7 +8059,7 @@
       <c r="A559" s="11"/>
       <c r="B559" s="11"/>
       <c r="C559" s="17" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="D559" s="11"/>
       <c r="E559" s="11"/>
@@ -8071,7 +8068,7 @@
       <c r="A560" s="11"/>
       <c r="B560" s="11"/>
       <c r="C560" s="17" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="D560" s="11"/>
       <c r="E560" s="11"/>
@@ -8080,7 +8077,7 @@
       <c r="A561" s="11"/>
       <c r="B561" s="11"/>
       <c r="C561" s="17" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="D561" s="11"/>
       <c r="E561" s="11"/>
@@ -8089,7 +8086,7 @@
       <c r="A562" s="11"/>
       <c r="B562" s="11"/>
       <c r="C562" s="17" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="D562" s="11"/>
       <c r="E562" s="11"/>
@@ -8098,7 +8095,7 @@
       <c r="A563" s="11"/>
       <c r="B563" s="11"/>
       <c r="C563" s="17" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="D563" s="11"/>
       <c r="E563" s="11"/>
@@ -8107,7 +8104,7 @@
       <c r="A564" s="11"/>
       <c r="B564" s="11"/>
       <c r="C564" s="17" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="D564" s="11"/>
       <c r="E564" s="11"/>
@@ -8116,7 +8113,7 @@
       <c r="A565" s="11"/>
       <c r="B565" s="11"/>
       <c r="C565" s="17" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="D565" s="11"/>
       <c r="E565" s="11"/>
@@ -8125,7 +8122,7 @@
       <c r="A566" s="11"/>
       <c r="B566" s="11"/>
       <c r="C566" s="17" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="D566" s="11"/>
       <c r="E566" s="11"/>
@@ -8134,7 +8131,7 @@
       <c r="A567" s="11"/>
       <c r="B567" s="11"/>
       <c r="C567" s="17" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="D567" s="11"/>
       <c r="E567" s="11"/>
@@ -8143,7 +8140,7 @@
       <c r="A568" s="11"/>
       <c r="B568" s="11"/>
       <c r="C568" s="17" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="D568" s="11"/>
       <c r="E568" s="11"/>
@@ -8152,7 +8149,7 @@
       <c r="A569" s="11"/>
       <c r="B569" s="11"/>
       <c r="C569" s="17" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="D569" s="11"/>
       <c r="E569" s="11"/>
@@ -8161,7 +8158,7 @@
       <c r="A570" s="11"/>
       <c r="B570" s="11"/>
       <c r="C570" s="17" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="D570" s="11"/>
       <c r="E570" s="11"/>
@@ -8170,7 +8167,7 @@
       <c r="A571" s="11"/>
       <c r="B571" s="11"/>
       <c r="C571" s="17" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="D571" s="11"/>
       <c r="E571" s="11"/>
@@ -8179,7 +8176,7 @@
       <c r="A572" s="11"/>
       <c r="B572" s="11"/>
       <c r="C572" s="17" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="D572" s="11"/>
       <c r="E572" s="11"/>
@@ -8188,7 +8185,7 @@
       <c r="A573" s="11"/>
       <c r="B573" s="11"/>
       <c r="C573" s="17" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="D573" s="11"/>
       <c r="E573" s="11"/>
@@ -8197,7 +8194,7 @@
       <c r="A574" s="11"/>
       <c r="B574" s="11"/>
       <c r="C574" s="17" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="D574" s="11"/>
       <c r="E574" s="11"/>
@@ -8206,7 +8203,7 @@
       <c r="A575" s="11"/>
       <c r="B575" s="11"/>
       <c r="C575" s="17" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="D575" s="11"/>
       <c r="E575" s="11"/>
@@ -8215,7 +8212,7 @@
       <c r="A576" s="11"/>
       <c r="B576" s="11"/>
       <c r="C576" s="17" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="D576" s="11"/>
       <c r="E576" s="11"/>
@@ -8224,7 +8221,7 @@
       <c r="A577" s="11"/>
       <c r="B577" s="11"/>
       <c r="C577" s="17" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="D577" s="11"/>
       <c r="E577" s="11"/>
@@ -8233,7 +8230,7 @@
       <c r="A578" s="11"/>
       <c r="B578" s="11"/>
       <c r="C578" s="17" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="D578" s="11"/>
       <c r="E578" s="11"/>
@@ -8242,7 +8239,7 @@
       <c r="A579" s="11"/>
       <c r="B579" s="11"/>
       <c r="C579" s="17" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="D579" s="11"/>
       <c r="E579" s="11"/>
@@ -8251,7 +8248,7 @@
       <c r="A580" s="11"/>
       <c r="B580" s="11"/>
       <c r="C580" s="17" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="D580" s="11"/>
       <c r="E580" s="11"/>
@@ -8260,7 +8257,7 @@
       <c r="A581" s="11"/>
       <c r="B581" s="11"/>
       <c r="C581" s="17" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="D581" s="11"/>
       <c r="E581" s="11"/>
@@ -8269,7 +8266,7 @@
       <c r="A582" s="11"/>
       <c r="B582" s="11"/>
       <c r="C582" s="17" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="D582" s="11"/>
       <c r="E582" s="11"/>
@@ -8278,7 +8275,7 @@
       <c r="A583" s="11"/>
       <c r="B583" s="11"/>
       <c r="C583" s="17" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="D583" s="11"/>
       <c r="E583" s="11"/>
@@ -8287,7 +8284,7 @@
       <c r="A584" s="11"/>
       <c r="B584" s="11"/>
       <c r="C584" s="17" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="D584" s="11"/>
       <c r="E584" s="11"/>
@@ -8296,7 +8293,7 @@
       <c r="A585" s="11"/>
       <c r="B585" s="11"/>
       <c r="C585" s="17" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="D585" s="11"/>
       <c r="E585" s="11"/>
@@ -8305,7 +8302,7 @@
       <c r="A586" s="11"/>
       <c r="B586" s="11"/>
       <c r="C586" s="17" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="D586" s="11"/>
       <c r="E586" s="11"/>
@@ -8314,7 +8311,7 @@
       <c r="A587" s="11"/>
       <c r="B587" s="11"/>
       <c r="C587" s="17" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="D587" s="11"/>
       <c r="E587" s="11"/>
@@ -8323,7 +8320,7 @@
       <c r="A588" s="11"/>
       <c r="B588" s="11"/>
       <c r="C588" s="17" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="D588" s="11"/>
       <c r="E588" s="11"/>
@@ -8332,7 +8329,7 @@
       <c r="A589" s="11"/>
       <c r="B589" s="11"/>
       <c r="C589" s="17" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="D589" s="11"/>
       <c r="E589" s="11"/>
@@ -8341,7 +8338,7 @@
       <c r="A590" s="11"/>
       <c r="B590" s="11"/>
       <c r="C590" s="17" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="D590" s="11"/>
       <c r="E590" s="11"/>
@@ -8350,7 +8347,7 @@
       <c r="A591" s="11"/>
       <c r="B591" s="11"/>
       <c r="C591" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="D591" s="11"/>
       <c r="E591" s="11"/>
@@ -8360,16 +8357,16 @@
         <v>131.0</v>
       </c>
       <c r="B592" s="8" t="s">
+        <v>405</v>
+      </c>
+      <c r="C592" s="64" t="s">
         <v>406</v>
-      </c>
-      <c r="C592" s="64" t="s">
-        <v>407</v>
       </c>
       <c r="D592" s="8" t="s">
         <v>91</v>
       </c>
       <c r="E592" s="6" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
     </row>
     <row r="593">
@@ -8377,16 +8374,16 @@
         <v>132.0</v>
       </c>
       <c r="B593" s="8" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="C593" s="8" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="D593" s="9" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="E593" s="72" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
     </row>
     <row r="594">
@@ -8394,10 +8391,10 @@
         <v>133.0</v>
       </c>
       <c r="B594" s="9" t="s">
+        <v>411</v>
+      </c>
+      <c r="C594" s="13" t="s">
         <v>412</v>
-      </c>
-      <c r="C594" s="13" t="s">
-        <v>413</v>
       </c>
       <c r="D594" s="9" t="s">
         <v>26</v>
@@ -8435,7 +8432,7 @@
       <c r="A598" s="11"/>
       <c r="B598" s="11"/>
       <c r="C598" s="20" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="D598" s="11"/>
       <c r="E598" s="11"/>
@@ -8445,13 +8442,13 @@
         <v>134.0</v>
       </c>
       <c r="B599" s="9" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C599" s="13" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="D599" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E599" s="72" t="s">
         <v>54</v>
@@ -8461,7 +8458,7 @@
       <c r="A600" s="11"/>
       <c r="B600" s="11"/>
       <c r="C600" s="13" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="D600" s="11"/>
       <c r="E600" s="11"/>
@@ -8471,13 +8468,13 @@
         <v>135.0</v>
       </c>
       <c r="B601" s="14" t="s">
+        <v>424</v>
+      </c>
+      <c r="C601" s="73" t="s">
         <v>425</v>
       </c>
-      <c r="C601" s="73" t="s">
-        <v>426</v>
-      </c>
       <c r="D601" s="15" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="E601" s="11"/>
     </row>
@@ -8485,7 +8482,7 @@
       <c r="A602" s="12"/>
       <c r="B602" s="19"/>
       <c r="C602" s="20" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="D602" s="21"/>
       <c r="E602" s="12"/>

</xml_diff>